<commit_message>
docs: Establish AI Collaboration Guidelines and align project docs
This is a major documentation update based on lessons learned from an intensive pair-programming experience with a generative AI.

- Establishes `99_ai_collaboration_guideline.md` as the project's "constitution" for human-AI interaction.
- Updates all key project documents (`README.md`, charter, coding standards, etc.) to reference and align with these new principles.
- This formalizes a robust, dialogue-based development protocol to prevent common AI pitfalls and enhance productivity.
</commit_message>
<xml_diff>
--- a/samples/excel_templates/simple-markdown-wbs-gantt-template.xlsx
+++ b/samples/excel_templates/simple-markdown-wbs-gantt-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\MD-WBS-Tools\samples\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A80089-656C-4CED-B503-4AAFAE5F9A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CFDAFC-E519-49DD-B904-18CB85BF5AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-29025" yWindow="11460" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -715,7 +715,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -924,13 +924,10 @@
     <xf numFmtId="9" fontId="14" fillId="3" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="2" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1648,11 +1645,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F0EA117-70A1-4F48-9934-ADBB69A804C6}">
   <dimension ref="A1:JH379"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="101" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="14" ySplit="4" topLeftCell="O5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="N1" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="V5" sqref="V5:X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="13.5" outlineLevelCol="1" x14ac:dyDescent="0.4"/>
@@ -1701,7 +1698,7 @@
       <c r="P1" s="6">
         <v>45796</v>
       </c>
-      <c r="Q1" s="70"/>
+      <c r="Q1" s="6"/>
       <c r="R1" s="7"/>
       <c r="S1" s="7"/>
       <c r="T1" s="7"/>
@@ -1732,9 +1729,9 @@
       </c>
       <c r="P2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45814</v>
-      </c>
-      <c r="Q2" s="70"/>
+        <v>45818</v>
+      </c>
+      <c r="Q2" s="6"/>
       <c r="R2" s="7"/>
       <c r="S2" s="7"/>
       <c r="T2" s="7"/>
@@ -1903,7 +1900,7 @@
       <c r="P3" s="54">
         <v>-1</v>
       </c>
-      <c r="Q3" s="71"/>
+      <c r="Q3" s="70"/>
       <c r="R3" s="55"/>
       <c r="S3" s="55"/>
       <c r="T3" s="55"/>
@@ -3940,7 +3937,7 @@
       </c>
       <c r="O5" s="34"/>
       <c r="P5" s="34"/>
-      <c r="Q5" s="72" t="str" cm="1">
+      <c r="Q5" s="71" t="str" cm="1">
         <f t="array" ref="Q5">IF(SUMPRODUCT(--(B5:E5&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -4004,7 +4001,7 @@
       </c>
       <c r="O6" s="34"/>
       <c r="P6" s="34"/>
-      <c r="Q6" s="72" t="str" cm="1">
+      <c r="Q6" s="71" t="str" cm="1">
         <f t="array" ref="Q6">IF(SUMPRODUCT(--(B6:E6&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -4068,7 +4065,7 @@
       </c>
       <c r="O7" s="34"/>
       <c r="P7" s="34"/>
-      <c r="Q7" s="72" t="str" cm="1">
+      <c r="Q7" s="71" t="str" cm="1">
         <f t="array" ref="Q7">IF(SUMPRODUCT(--(B7:E7&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -4132,7 +4129,7 @@
       </c>
       <c r="O8" s="34"/>
       <c r="P8" s="34"/>
-      <c r="Q8" s="72" t="str" cm="1">
+      <c r="Q8" s="71" t="str" cm="1">
         <f t="array" ref="Q8">IF(SUMPRODUCT(--(B8:E8&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -4196,7 +4193,7 @@
       </c>
       <c r="O9" s="34"/>
       <c r="P9" s="34"/>
-      <c r="Q9" s="72" t="str" cm="1">
+      <c r="Q9" s="71" t="str" cm="1">
         <f t="array" ref="Q9">IF(SUMPRODUCT(--(B9:E9&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -4260,7 +4257,7 @@
       </c>
       <c r="O10" s="34"/>
       <c r="P10" s="34"/>
-      <c r="Q10" s="72" t="str" cm="1">
+      <c r="Q10" s="71" t="str" cm="1">
         <f t="array" ref="Q10">IF(SUMPRODUCT(--(B10:E10&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -4324,7 +4321,7 @@
       </c>
       <c r="O11" s="34"/>
       <c r="P11" s="34"/>
-      <c r="Q11" s="72" t="str" cm="1">
+      <c r="Q11" s="71" t="str" cm="1">
         <f t="array" ref="Q11">IF(SUMPRODUCT(--(B11:E11&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -4388,7 +4385,7 @@
       </c>
       <c r="O12" s="34"/>
       <c r="P12" s="34"/>
-      <c r="Q12" s="72" t="str" cm="1">
+      <c r="Q12" s="71" t="str" cm="1">
         <f t="array" ref="Q12">IF(SUMPRODUCT(--(B12:E12&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -4452,7 +4449,7 @@
       </c>
       <c r="O13" s="34"/>
       <c r="P13" s="34"/>
-      <c r="Q13" s="72" t="str" cm="1">
+      <c r="Q13" s="71" t="str" cm="1">
         <f t="array" ref="Q13">IF(SUMPRODUCT(--(B13:E13&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -4516,7 +4513,7 @@
       </c>
       <c r="O14" s="34"/>
       <c r="P14" s="34"/>
-      <c r="Q14" s="72" t="str" cm="1">
+      <c r="Q14" s="71" t="str" cm="1">
         <f t="array" ref="Q14">IF(SUMPRODUCT(--(B14:E14&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -4580,7 +4577,7 @@
       </c>
       <c r="O15" s="34"/>
       <c r="P15" s="34"/>
-      <c r="Q15" s="72" t="str" cm="1">
+      <c r="Q15" s="71" t="str" cm="1">
         <f t="array" ref="Q15">IF(SUMPRODUCT(--(B15:E15&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -4644,7 +4641,7 @@
       </c>
       <c r="O16" s="34"/>
       <c r="P16" s="34"/>
-      <c r="Q16" s="72" t="str" cm="1">
+      <c r="Q16" s="71" t="str" cm="1">
         <f t="array" ref="Q16">IF(SUMPRODUCT(--(B16:E16&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -4708,7 +4705,7 @@
       </c>
       <c r="O17" s="34"/>
       <c r="P17" s="34"/>
-      <c r="Q17" s="72" t="str" cm="1">
+      <c r="Q17" s="71" t="str" cm="1">
         <f t="array" ref="Q17">IF(SUMPRODUCT(--(B17:E17&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -4772,7 +4769,7 @@
       </c>
       <c r="O18" s="34"/>
       <c r="P18" s="34"/>
-      <c r="Q18" s="72" t="str" cm="1">
+      <c r="Q18" s="71" t="str" cm="1">
         <f t="array" ref="Q18">IF(SUMPRODUCT(--(B18:E18&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -4836,7 +4833,7 @@
       </c>
       <c r="O19" s="34"/>
       <c r="P19" s="34"/>
-      <c r="Q19" s="72" t="str" cm="1">
+      <c r="Q19" s="71" t="str" cm="1">
         <f t="array" ref="Q19">IF(SUMPRODUCT(--(B19:E19&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -4900,7 +4897,7 @@
       </c>
       <c r="O20" s="34"/>
       <c r="P20" s="34"/>
-      <c r="Q20" s="72" t="str" cm="1">
+      <c r="Q20" s="71" t="str" cm="1">
         <f t="array" ref="Q20">IF(SUMPRODUCT(--(B20:E20&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -4964,7 +4961,7 @@
       </c>
       <c r="O21" s="34"/>
       <c r="P21" s="34"/>
-      <c r="Q21" s="72" t="str" cm="1">
+      <c r="Q21" s="71" t="str" cm="1">
         <f t="array" ref="Q21">IF(SUMPRODUCT(--(B21:E21&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -5028,7 +5025,7 @@
       </c>
       <c r="O22" s="34"/>
       <c r="P22" s="34"/>
-      <c r="Q22" s="72" t="str" cm="1">
+      <c r="Q22" s="71" t="str" cm="1">
         <f t="array" ref="Q22">IF(SUMPRODUCT(--(B22:E22&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -5092,7 +5089,7 @@
       </c>
       <c r="O23" s="34"/>
       <c r="P23" s="34"/>
-      <c r="Q23" s="72" t="str" cm="1">
+      <c r="Q23" s="71" t="str" cm="1">
         <f t="array" ref="Q23">IF(SUMPRODUCT(--(B23:E23&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -5156,7 +5153,7 @@
       </c>
       <c r="O24" s="34"/>
       <c r="P24" s="34"/>
-      <c r="Q24" s="72" t="str" cm="1">
+      <c r="Q24" s="71" t="str" cm="1">
         <f t="array" ref="Q24">IF(SUMPRODUCT(--(B24:E24&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -5220,7 +5217,7 @@
       </c>
       <c r="O25" s="34"/>
       <c r="P25" s="34"/>
-      <c r="Q25" s="72" t="str" cm="1">
+      <c r="Q25" s="71" t="str" cm="1">
         <f t="array" ref="Q25">IF(SUMPRODUCT(--(B25:E25&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -5284,7 +5281,7 @@
       </c>
       <c r="O26" s="34"/>
       <c r="P26" s="34"/>
-      <c r="Q26" s="72" t="str" cm="1">
+      <c r="Q26" s="71" t="str" cm="1">
         <f t="array" ref="Q26">IF(SUMPRODUCT(--(B26:E26&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -5348,7 +5345,7 @@
       </c>
       <c r="O27" s="34"/>
       <c r="P27" s="34"/>
-      <c r="Q27" s="72" t="str" cm="1">
+      <c r="Q27" s="71" t="str" cm="1">
         <f t="array" ref="Q27">IF(SUMPRODUCT(--(B27:E27&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -5412,7 +5409,7 @@
       </c>
       <c r="O28" s="34"/>
       <c r="P28" s="34"/>
-      <c r="Q28" s="72" t="str" cm="1">
+      <c r="Q28" s="71" t="str" cm="1">
         <f t="array" ref="Q28">IF(SUMPRODUCT(--(B28:E28&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -5476,7 +5473,7 @@
       </c>
       <c r="O29" s="34"/>
       <c r="P29" s="34"/>
-      <c r="Q29" s="72" t="str" cm="1">
+      <c r="Q29" s="71" t="str" cm="1">
         <f t="array" ref="Q29">IF(SUMPRODUCT(--(B29:E29&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -5540,7 +5537,7 @@
       </c>
       <c r="O30" s="34"/>
       <c r="P30" s="34"/>
-      <c r="Q30" s="72" t="str" cm="1">
+      <c r="Q30" s="71" t="str" cm="1">
         <f t="array" ref="Q30">IF(SUMPRODUCT(--(B30:E30&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -5604,7 +5601,7 @@
       </c>
       <c r="O31" s="34"/>
       <c r="P31" s="34"/>
-      <c r="Q31" s="72" t="str" cm="1">
+      <c r="Q31" s="71" t="str" cm="1">
         <f t="array" ref="Q31">IF(SUMPRODUCT(--(B31:E31&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -5668,7 +5665,7 @@
       </c>
       <c r="O32" s="34"/>
       <c r="P32" s="34"/>
-      <c r="Q32" s="72" t="str" cm="1">
+      <c r="Q32" s="71" t="str" cm="1">
         <f t="array" ref="Q32">IF(SUMPRODUCT(--(B32:E32&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -5732,7 +5729,7 @@
       </c>
       <c r="O33" s="34"/>
       <c r="P33" s="34"/>
-      <c r="Q33" s="72" t="str" cm="1">
+      <c r="Q33" s="71" t="str" cm="1">
         <f t="array" ref="Q33">IF(SUMPRODUCT(--(B33:E33&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -5796,7 +5793,7 @@
       </c>
       <c r="O34" s="34"/>
       <c r="P34" s="34"/>
-      <c r="Q34" s="72" t="str" cm="1">
+      <c r="Q34" s="71" t="str" cm="1">
         <f t="array" ref="Q34">IF(SUMPRODUCT(--(B34:E34&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -5860,7 +5857,7 @@
       </c>
       <c r="O35" s="34"/>
       <c r="P35" s="34"/>
-      <c r="Q35" s="72" t="str" cm="1">
+      <c r="Q35" s="71" t="str" cm="1">
         <f t="array" ref="Q35">IF(SUMPRODUCT(--(B35:E35&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -5924,7 +5921,7 @@
       </c>
       <c r="O36" s="34"/>
       <c r="P36" s="34"/>
-      <c r="Q36" s="72" t="str" cm="1">
+      <c r="Q36" s="71" t="str" cm="1">
         <f t="array" ref="Q36">IF(SUMPRODUCT(--(B36:E36&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -5988,7 +5985,7 @@
       </c>
       <c r="O37" s="34"/>
       <c r="P37" s="34"/>
-      <c r="Q37" s="72" t="str" cm="1">
+      <c r="Q37" s="71" t="str" cm="1">
         <f t="array" ref="Q37">IF(SUMPRODUCT(--(B37:E37&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -6052,7 +6049,7 @@
       </c>
       <c r="O38" s="34"/>
       <c r="P38" s="34"/>
-      <c r="Q38" s="72" t="str" cm="1">
+      <c r="Q38" s="71" t="str" cm="1">
         <f t="array" ref="Q38">IF(SUMPRODUCT(--(B38:E38&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -6116,7 +6113,7 @@
       </c>
       <c r="O39" s="34"/>
       <c r="P39" s="34"/>
-      <c r="Q39" s="72" t="str" cm="1">
+      <c r="Q39" s="71" t="str" cm="1">
         <f t="array" ref="Q39">IF(SUMPRODUCT(--(B39:E39&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -6180,7 +6177,7 @@
       </c>
       <c r="O40" s="34"/>
       <c r="P40" s="34"/>
-      <c r="Q40" s="72" t="str" cm="1">
+      <c r="Q40" s="71" t="str" cm="1">
         <f t="array" ref="Q40">IF(SUMPRODUCT(--(B40:E40&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -6244,7 +6241,7 @@
       </c>
       <c r="O41" s="34"/>
       <c r="P41" s="34"/>
-      <c r="Q41" s="72" t="str" cm="1">
+      <c r="Q41" s="71" t="str" cm="1">
         <f t="array" ref="Q41">IF(SUMPRODUCT(--(B41:E41&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -6308,7 +6305,7 @@
       </c>
       <c r="O42" s="34"/>
       <c r="P42" s="34"/>
-      <c r="Q42" s="72" t="str" cm="1">
+      <c r="Q42" s="71" t="str" cm="1">
         <f t="array" ref="Q42">IF(SUMPRODUCT(--(B42:E42&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -6372,7 +6369,7 @@
       </c>
       <c r="O43" s="34"/>
       <c r="P43" s="34"/>
-      <c r="Q43" s="72" t="str" cm="1">
+      <c r="Q43" s="71" t="str" cm="1">
         <f t="array" ref="Q43">IF(SUMPRODUCT(--(B43:E43&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -6436,7 +6433,7 @@
       </c>
       <c r="O44" s="34"/>
       <c r="P44" s="34"/>
-      <c r="Q44" s="72" t="str" cm="1">
+      <c r="Q44" s="71" t="str" cm="1">
         <f t="array" ref="Q44">IF(SUMPRODUCT(--(B44:E44&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -6500,7 +6497,7 @@
       </c>
       <c r="O45" s="34"/>
       <c r="P45" s="34"/>
-      <c r="Q45" s="72" t="str" cm="1">
+      <c r="Q45" s="71" t="str" cm="1">
         <f t="array" ref="Q45">IF(SUMPRODUCT(--(B45:E45&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -6564,7 +6561,7 @@
       </c>
       <c r="O46" s="34"/>
       <c r="P46" s="34"/>
-      <c r="Q46" s="72" t="str" cm="1">
+      <c r="Q46" s="71" t="str" cm="1">
         <f t="array" ref="Q46">IF(SUMPRODUCT(--(B46:E46&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -6628,7 +6625,7 @@
       </c>
       <c r="O47" s="34"/>
       <c r="P47" s="34"/>
-      <c r="Q47" s="72" t="str" cm="1">
+      <c r="Q47" s="71" t="str" cm="1">
         <f t="array" ref="Q47">IF(SUMPRODUCT(--(B47:E47&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -6692,7 +6689,7 @@
       </c>
       <c r="O48" s="34"/>
       <c r="P48" s="34"/>
-      <c r="Q48" s="72" t="str" cm="1">
+      <c r="Q48" s="71" t="str" cm="1">
         <f t="array" ref="Q48">IF(SUMPRODUCT(--(B48:E48&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -6756,7 +6753,7 @@
       </c>
       <c r="O49" s="34"/>
       <c r="P49" s="34"/>
-      <c r="Q49" s="72" t="str" cm="1">
+      <c r="Q49" s="71" t="str" cm="1">
         <f t="array" ref="Q49">IF(SUMPRODUCT(--(B49:E49&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -6820,7 +6817,7 @@
       </c>
       <c r="O50" s="34"/>
       <c r="P50" s="34"/>
-      <c r="Q50" s="72" t="str" cm="1">
+      <c r="Q50" s="71" t="str" cm="1">
         <f t="array" ref="Q50">IF(SUMPRODUCT(--(B50:E50&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -6884,7 +6881,7 @@
       </c>
       <c r="O51" s="34"/>
       <c r="P51" s="34"/>
-      <c r="Q51" s="72" t="str" cm="1">
+      <c r="Q51" s="71" t="str" cm="1">
         <f t="array" ref="Q51">IF(SUMPRODUCT(--(B51:E51&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -6948,7 +6945,7 @@
       </c>
       <c r="O52" s="34"/>
       <c r="P52" s="34"/>
-      <c r="Q52" s="72" t="str" cm="1">
+      <c r="Q52" s="71" t="str" cm="1">
         <f t="array" ref="Q52">IF(SUMPRODUCT(--(B52:E52&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -7012,7 +7009,7 @@
       </c>
       <c r="O53" s="34"/>
       <c r="P53" s="34"/>
-      <c r="Q53" s="72" t="str" cm="1">
+      <c r="Q53" s="71" t="str" cm="1">
         <f t="array" ref="Q53">IF(SUMPRODUCT(--(B53:E53&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -7076,7 +7073,7 @@
       </c>
       <c r="O54" s="34"/>
       <c r="P54" s="34"/>
-      <c r="Q54" s="72" t="str" cm="1">
+      <c r="Q54" s="71" t="str" cm="1">
         <f t="array" ref="Q54">IF(SUMPRODUCT(--(B54:E54&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -7140,7 +7137,7 @@
       </c>
       <c r="O55" s="34"/>
       <c r="P55" s="34"/>
-      <c r="Q55" s="72" t="str" cm="1">
+      <c r="Q55" s="71" t="str" cm="1">
         <f t="array" ref="Q55">IF(SUMPRODUCT(--(B55:E55&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -7204,7 +7201,7 @@
       </c>
       <c r="O56" s="34"/>
       <c r="P56" s="34"/>
-      <c r="Q56" s="72" t="str" cm="1">
+      <c r="Q56" s="71" t="str" cm="1">
         <f t="array" ref="Q56">IF(SUMPRODUCT(--(B56:E56&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -7268,7 +7265,7 @@
       </c>
       <c r="O57" s="34"/>
       <c r="P57" s="34"/>
-      <c r="Q57" s="72" t="str" cm="1">
+      <c r="Q57" s="71" t="str" cm="1">
         <f t="array" ref="Q57">IF(SUMPRODUCT(--(B57:E57&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -7332,7 +7329,7 @@
       </c>
       <c r="O58" s="34"/>
       <c r="P58" s="34"/>
-      <c r="Q58" s="72" t="str" cm="1">
+      <c r="Q58" s="71" t="str" cm="1">
         <f t="array" ref="Q58">IF(SUMPRODUCT(--(B58:E58&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -7396,7 +7393,7 @@
       </c>
       <c r="O59" s="34"/>
       <c r="P59" s="34"/>
-      <c r="Q59" s="72" t="str" cm="1">
+      <c r="Q59" s="71" t="str" cm="1">
         <f t="array" ref="Q59">IF(SUMPRODUCT(--(B59:E59&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -7460,7 +7457,7 @@
       </c>
       <c r="O60" s="34"/>
       <c r="P60" s="34"/>
-      <c r="Q60" s="72" t="str" cm="1">
+      <c r="Q60" s="71" t="str" cm="1">
         <f t="array" ref="Q60">IF(SUMPRODUCT(--(B60:E60&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -7524,7 +7521,7 @@
       </c>
       <c r="O61" s="34"/>
       <c r="P61" s="34"/>
-      <c r="Q61" s="72" t="str" cm="1">
+      <c r="Q61" s="71" t="str" cm="1">
         <f t="array" ref="Q61">IF(SUMPRODUCT(--(B61:E61&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -7588,7 +7585,7 @@
       </c>
       <c r="O62" s="34"/>
       <c r="P62" s="34"/>
-      <c r="Q62" s="72" t="str" cm="1">
+      <c r="Q62" s="71" t="str" cm="1">
         <f t="array" ref="Q62">IF(SUMPRODUCT(--(B62:E62&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -7652,7 +7649,7 @@
       </c>
       <c r="O63" s="34"/>
       <c r="P63" s="34"/>
-      <c r="Q63" s="72" t="str" cm="1">
+      <c r="Q63" s="71" t="str" cm="1">
         <f t="array" ref="Q63">IF(SUMPRODUCT(--(B63:E63&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -7716,7 +7713,7 @@
       </c>
       <c r="O64" s="34"/>
       <c r="P64" s="34"/>
-      <c r="Q64" s="72" t="str" cm="1">
+      <c r="Q64" s="71" t="str" cm="1">
         <f t="array" ref="Q64">IF(SUMPRODUCT(--(B64:E64&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -7780,7 +7777,7 @@
       </c>
       <c r="O65" s="34"/>
       <c r="P65" s="34"/>
-      <c r="Q65" s="72" t="str" cm="1">
+      <c r="Q65" s="71" t="str" cm="1">
         <f t="array" ref="Q65">IF(SUMPRODUCT(--(B65:E65&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -7844,7 +7841,7 @@
       </c>
       <c r="O66" s="34"/>
       <c r="P66" s="34"/>
-      <c r="Q66" s="72" t="str" cm="1">
+      <c r="Q66" s="71" t="str" cm="1">
         <f t="array" ref="Q66">IF(SUMPRODUCT(--(B66:E66&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -7908,7 +7905,7 @@
       </c>
       <c r="O67" s="34"/>
       <c r="P67" s="34"/>
-      <c r="Q67" s="72" t="str" cm="1">
+      <c r="Q67" s="71" t="str" cm="1">
         <f t="array" ref="Q67">IF(SUMPRODUCT(--(B67:E67&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -7972,7 +7969,7 @@
       </c>
       <c r="O68" s="34"/>
       <c r="P68" s="34"/>
-      <c r="Q68" s="72" t="str" cm="1">
+      <c r="Q68" s="71" t="str" cm="1">
         <f t="array" ref="Q68">IF(SUMPRODUCT(--(B68:E68&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -8036,7 +8033,7 @@
       </c>
       <c r="O69" s="34"/>
       <c r="P69" s="34"/>
-      <c r="Q69" s="72" t="str" cm="1">
+      <c r="Q69" s="71" t="str" cm="1">
         <f t="array" ref="Q69">IF(SUMPRODUCT(--(B69:E69&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -8100,7 +8097,7 @@
       </c>
       <c r="O70" s="34"/>
       <c r="P70" s="34"/>
-      <c r="Q70" s="72" t="str" cm="1">
+      <c r="Q70" s="71" t="str" cm="1">
         <f t="array" ref="Q70">IF(SUMPRODUCT(--(B70:E70&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -8164,7 +8161,7 @@
       </c>
       <c r="O71" s="34"/>
       <c r="P71" s="34"/>
-      <c r="Q71" s="72" t="str" cm="1">
+      <c r="Q71" s="71" t="str" cm="1">
         <f t="array" ref="Q71">IF(SUMPRODUCT(--(B71:E71&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -8228,7 +8225,7 @@
       </c>
       <c r="O72" s="34"/>
       <c r="P72" s="34"/>
-      <c r="Q72" s="72" t="str" cm="1">
+      <c r="Q72" s="71" t="str" cm="1">
         <f t="array" ref="Q72">IF(SUMPRODUCT(--(B72:E72&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -8292,7 +8289,7 @@
       </c>
       <c r="O73" s="34"/>
       <c r="P73" s="34"/>
-      <c r="Q73" s="72" t="str" cm="1">
+      <c r="Q73" s="71" t="str" cm="1">
         <f t="array" ref="Q73">IF(SUMPRODUCT(--(B73:E73&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -8356,7 +8353,7 @@
       </c>
       <c r="O74" s="34"/>
       <c r="P74" s="34"/>
-      <c r="Q74" s="72" t="str" cm="1">
+      <c r="Q74" s="71" t="str" cm="1">
         <f t="array" ref="Q74">IF(SUMPRODUCT(--(B74:E74&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -8420,7 +8417,7 @@
       </c>
       <c r="O75" s="34"/>
       <c r="P75" s="34"/>
-      <c r="Q75" s="72" t="str" cm="1">
+      <c r="Q75" s="71" t="str" cm="1">
         <f t="array" ref="Q75">IF(SUMPRODUCT(--(B75:E75&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -8484,7 +8481,7 @@
       </c>
       <c r="O76" s="34"/>
       <c r="P76" s="34"/>
-      <c r="Q76" s="72" t="str" cm="1">
+      <c r="Q76" s="71" t="str" cm="1">
         <f t="array" ref="Q76">IF(SUMPRODUCT(--(B76:E76&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -8548,7 +8545,7 @@
       </c>
       <c r="O77" s="34"/>
       <c r="P77" s="34"/>
-      <c r="Q77" s="72" t="str" cm="1">
+      <c r="Q77" s="71" t="str" cm="1">
         <f t="array" ref="Q77">IF(SUMPRODUCT(--(B77:E77&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -8612,7 +8609,7 @@
       </c>
       <c r="O78" s="34"/>
       <c r="P78" s="34"/>
-      <c r="Q78" s="72" t="str" cm="1">
+      <c r="Q78" s="71" t="str" cm="1">
         <f t="array" ref="Q78">IF(SUMPRODUCT(--(B78:E78&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -8676,7 +8673,7 @@
       </c>
       <c r="O79" s="34"/>
       <c r="P79" s="34"/>
-      <c r="Q79" s="72" t="str" cm="1">
+      <c r="Q79" s="71" t="str" cm="1">
         <f t="array" ref="Q79">IF(SUMPRODUCT(--(B79:E79&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -8740,7 +8737,7 @@
       </c>
       <c r="O80" s="34"/>
       <c r="P80" s="34"/>
-      <c r="Q80" s="72" t="str" cm="1">
+      <c r="Q80" s="71" t="str" cm="1">
         <f t="array" ref="Q80">IF(SUMPRODUCT(--(B80:E80&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -8804,7 +8801,7 @@
       </c>
       <c r="O81" s="34"/>
       <c r="P81" s="34"/>
-      <c r="Q81" s="72" t="str" cm="1">
+      <c r="Q81" s="71" t="str" cm="1">
         <f t="array" ref="Q81">IF(SUMPRODUCT(--(B81:E81&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -8868,7 +8865,7 @@
       </c>
       <c r="O82" s="34"/>
       <c r="P82" s="34"/>
-      <c r="Q82" s="72" t="str" cm="1">
+      <c r="Q82" s="71" t="str" cm="1">
         <f t="array" ref="Q82">IF(SUMPRODUCT(--(B82:E82&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -8932,7 +8929,7 @@
       </c>
       <c r="O83" s="34"/>
       <c r="P83" s="34"/>
-      <c r="Q83" s="72" t="str" cm="1">
+      <c r="Q83" s="71" t="str" cm="1">
         <f t="array" ref="Q83">IF(SUMPRODUCT(--(B83:E83&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -8996,7 +8993,7 @@
       </c>
       <c r="O84" s="34"/>
       <c r="P84" s="34"/>
-      <c r="Q84" s="72" t="str" cm="1">
+      <c r="Q84" s="71" t="str" cm="1">
         <f t="array" ref="Q84">IF(SUMPRODUCT(--(B84:E84&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -9060,7 +9057,7 @@
       </c>
       <c r="O85" s="34"/>
       <c r="P85" s="34"/>
-      <c r="Q85" s="72" t="str" cm="1">
+      <c r="Q85" s="71" t="str" cm="1">
         <f t="array" ref="Q85">IF(SUMPRODUCT(--(B85:E85&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -9124,7 +9121,7 @@
       </c>
       <c r="O86" s="34"/>
       <c r="P86" s="34"/>
-      <c r="Q86" s="72" t="str" cm="1">
+      <c r="Q86" s="71" t="str" cm="1">
         <f t="array" ref="Q86">IF(SUMPRODUCT(--(B86:E86&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -9188,7 +9185,7 @@
       </c>
       <c r="O87" s="34"/>
       <c r="P87" s="34"/>
-      <c r="Q87" s="72" t="str" cm="1">
+      <c r="Q87" s="71" t="str" cm="1">
         <f t="array" ref="Q87">IF(SUMPRODUCT(--(B87:E87&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -9252,7 +9249,7 @@
       </c>
       <c r="O88" s="34"/>
       <c r="P88" s="34"/>
-      <c r="Q88" s="72" t="str" cm="1">
+      <c r="Q88" s="71" t="str" cm="1">
         <f t="array" ref="Q88">IF(SUMPRODUCT(--(B88:E88&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -9316,7 +9313,7 @@
       </c>
       <c r="O89" s="34"/>
       <c r="P89" s="34"/>
-      <c r="Q89" s="72" t="str" cm="1">
+      <c r="Q89" s="71" t="str" cm="1">
         <f t="array" ref="Q89">IF(SUMPRODUCT(--(B89:E89&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -9380,7 +9377,7 @@
       </c>
       <c r="O90" s="34"/>
       <c r="P90" s="34"/>
-      <c r="Q90" s="72" t="str" cm="1">
+      <c r="Q90" s="71" t="str" cm="1">
         <f t="array" ref="Q90">IF(SUMPRODUCT(--(B90:E90&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -9444,7 +9441,7 @@
       </c>
       <c r="O91" s="34"/>
       <c r="P91" s="34"/>
-      <c r="Q91" s="72" t="str" cm="1">
+      <c r="Q91" s="71" t="str" cm="1">
         <f t="array" ref="Q91">IF(SUMPRODUCT(--(B91:E91&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -9508,7 +9505,7 @@
       </c>
       <c r="O92" s="34"/>
       <c r="P92" s="34"/>
-      <c r="Q92" s="72" t="str" cm="1">
+      <c r="Q92" s="71" t="str" cm="1">
         <f t="array" ref="Q92">IF(SUMPRODUCT(--(B92:E92&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -9572,7 +9569,7 @@
       </c>
       <c r="O93" s="34"/>
       <c r="P93" s="34"/>
-      <c r="Q93" s="72" t="str" cm="1">
+      <c r="Q93" s="71" t="str" cm="1">
         <f t="array" ref="Q93">IF(SUMPRODUCT(--(B93:E93&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -9636,7 +9633,7 @@
       </c>
       <c r="O94" s="34"/>
       <c r="P94" s="34"/>
-      <c r="Q94" s="72" t="str" cm="1">
+      <c r="Q94" s="71" t="str" cm="1">
         <f t="array" ref="Q94">IF(SUMPRODUCT(--(B94:E94&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -9700,7 +9697,7 @@
       </c>
       <c r="O95" s="34"/>
       <c r="P95" s="34"/>
-      <c r="Q95" s="72" t="str" cm="1">
+      <c r="Q95" s="71" t="str" cm="1">
         <f t="array" ref="Q95">IF(SUMPRODUCT(--(B95:E95&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -9764,7 +9761,7 @@
       </c>
       <c r="O96" s="34"/>
       <c r="P96" s="34"/>
-      <c r="Q96" s="72" t="str" cm="1">
+      <c r="Q96" s="71" t="str" cm="1">
         <f t="array" ref="Q96">IF(SUMPRODUCT(--(B96:E96&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -9828,7 +9825,7 @@
       </c>
       <c r="O97" s="34"/>
       <c r="P97" s="34"/>
-      <c r="Q97" s="72" t="str" cm="1">
+      <c r="Q97" s="71" t="str" cm="1">
         <f t="array" ref="Q97">IF(SUMPRODUCT(--(B97:E97&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -9892,7 +9889,7 @@
       </c>
       <c r="O98" s="34"/>
       <c r="P98" s="34"/>
-      <c r="Q98" s="72" t="str" cm="1">
+      <c r="Q98" s="71" t="str" cm="1">
         <f t="array" ref="Q98">IF(SUMPRODUCT(--(B98:E98&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -9956,7 +9953,7 @@
       </c>
       <c r="O99" s="34"/>
       <c r="P99" s="34"/>
-      <c r="Q99" s="72" t="str" cm="1">
+      <c r="Q99" s="71" t="str" cm="1">
         <f t="array" ref="Q99">IF(SUMPRODUCT(--(B99:E99&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -10020,7 +10017,7 @@
       </c>
       <c r="O100" s="34"/>
       <c r="P100" s="34"/>
-      <c r="Q100" s="72" t="str" cm="1">
+      <c r="Q100" s="71" t="str" cm="1">
         <f t="array" ref="Q100">IF(SUMPRODUCT(--(B100:E100&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -10084,7 +10081,7 @@
       </c>
       <c r="O101" s="34"/>
       <c r="P101" s="34"/>
-      <c r="Q101" s="72" t="str" cm="1">
+      <c r="Q101" s="71" t="str" cm="1">
         <f t="array" ref="Q101">IF(SUMPRODUCT(--(B101:E101&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -10148,7 +10145,7 @@
       </c>
       <c r="O102" s="34"/>
       <c r="P102" s="34"/>
-      <c r="Q102" s="72" t="str" cm="1">
+      <c r="Q102" s="71" t="str" cm="1">
         <f t="array" ref="Q102">IF(SUMPRODUCT(--(B102:E102&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -10212,7 +10209,7 @@
       </c>
       <c r="O103" s="34"/>
       <c r="P103" s="34"/>
-      <c r="Q103" s="72" t="str" cm="1">
+      <c r="Q103" s="71" t="str" cm="1">
         <f t="array" ref="Q103">IF(SUMPRODUCT(--(B103:E103&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -10276,7 +10273,7 @@
       </c>
       <c r="O104" s="34"/>
       <c r="P104" s="34"/>
-      <c r="Q104" s="72" t="str" cm="1">
+      <c r="Q104" s="71" t="str" cm="1">
         <f t="array" ref="Q104">IF(SUMPRODUCT(--(B104:E104&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -10340,7 +10337,7 @@
       </c>
       <c r="O105" s="34"/>
       <c r="P105" s="34"/>
-      <c r="Q105" s="72" t="str" cm="1">
+      <c r="Q105" s="71" t="str" cm="1">
         <f t="array" ref="Q105">IF(SUMPRODUCT(--(B105:E105&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -10404,7 +10401,7 @@
       </c>
       <c r="O106" s="34"/>
       <c r="P106" s="34"/>
-      <c r="Q106" s="72" t="str" cm="1">
+      <c r="Q106" s="71" t="str" cm="1">
         <f t="array" ref="Q106">IF(SUMPRODUCT(--(B106:E106&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -10468,7 +10465,7 @@
       </c>
       <c r="O107" s="34"/>
       <c r="P107" s="34"/>
-      <c r="Q107" s="72" t="str" cm="1">
+      <c r="Q107" s="71" t="str" cm="1">
         <f t="array" ref="Q107">IF(SUMPRODUCT(--(B107:E107&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -10532,7 +10529,7 @@
       </c>
       <c r="O108" s="34"/>
       <c r="P108" s="34"/>
-      <c r="Q108" s="72" t="str" cm="1">
+      <c r="Q108" s="71" t="str" cm="1">
         <f t="array" ref="Q108">IF(SUMPRODUCT(--(B108:E108&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -10596,7 +10593,7 @@
       </c>
       <c r="O109" s="34"/>
       <c r="P109" s="34"/>
-      <c r="Q109" s="72" t="str" cm="1">
+      <c r="Q109" s="71" t="str" cm="1">
         <f t="array" ref="Q109">IF(SUMPRODUCT(--(B109:E109&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -10660,7 +10657,7 @@
       </c>
       <c r="O110" s="34"/>
       <c r="P110" s="34"/>
-      <c r="Q110" s="72" t="str" cm="1">
+      <c r="Q110" s="71" t="str" cm="1">
         <f t="array" ref="Q110">IF(SUMPRODUCT(--(B110:E110&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -10724,7 +10721,7 @@
       </c>
       <c r="O111" s="34"/>
       <c r="P111" s="34"/>
-      <c r="Q111" s="72" t="str" cm="1">
+      <c r="Q111" s="71" t="str" cm="1">
         <f t="array" ref="Q111">IF(SUMPRODUCT(--(B111:E111&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -10788,7 +10785,7 @@
       </c>
       <c r="O112" s="34"/>
       <c r="P112" s="34"/>
-      <c r="Q112" s="72" t="str" cm="1">
+      <c r="Q112" s="71" t="str" cm="1">
         <f t="array" ref="Q112">IF(SUMPRODUCT(--(B112:E112&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -10852,7 +10849,7 @@
       </c>
       <c r="O113" s="34"/>
       <c r="P113" s="34"/>
-      <c r="Q113" s="72" t="str" cm="1">
+      <c r="Q113" s="71" t="str" cm="1">
         <f t="array" ref="Q113">IF(SUMPRODUCT(--(B113:E113&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -10916,7 +10913,7 @@
       </c>
       <c r="O114" s="34"/>
       <c r="P114" s="34"/>
-      <c r="Q114" s="72" t="str" cm="1">
+      <c r="Q114" s="71" t="str" cm="1">
         <f t="array" ref="Q114">IF(SUMPRODUCT(--(B114:E114&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -10980,7 +10977,7 @@
       </c>
       <c r="O115" s="34"/>
       <c r="P115" s="34"/>
-      <c r="Q115" s="72" t="str" cm="1">
+      <c r="Q115" s="71" t="str" cm="1">
         <f t="array" ref="Q115">IF(SUMPRODUCT(--(B115:E115&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -11044,7 +11041,7 @@
       </c>
       <c r="O116" s="34"/>
       <c r="P116" s="34"/>
-      <c r="Q116" s="72" t="str" cm="1">
+      <c r="Q116" s="71" t="str" cm="1">
         <f t="array" ref="Q116">IF(SUMPRODUCT(--(B116:E116&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -11108,7 +11105,7 @@
       </c>
       <c r="O117" s="34"/>
       <c r="P117" s="34"/>
-      <c r="Q117" s="72" t="str" cm="1">
+      <c r="Q117" s="71" t="str" cm="1">
         <f t="array" ref="Q117">IF(SUMPRODUCT(--(B117:E117&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -11172,7 +11169,7 @@
       </c>
       <c r="O118" s="34"/>
       <c r="P118" s="34"/>
-      <c r="Q118" s="72" t="str" cm="1">
+      <c r="Q118" s="71" t="str" cm="1">
         <f t="array" ref="Q118">IF(SUMPRODUCT(--(B118:E118&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -11236,7 +11233,7 @@
       </c>
       <c r="O119" s="34"/>
       <c r="P119" s="34"/>
-      <c r="Q119" s="72" t="str" cm="1">
+      <c r="Q119" s="71" t="str" cm="1">
         <f t="array" ref="Q119">IF(SUMPRODUCT(--(B119:E119&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -11300,7 +11297,7 @@
       </c>
       <c r="O120" s="34"/>
       <c r="P120" s="34"/>
-      <c r="Q120" s="72" t="str" cm="1">
+      <c r="Q120" s="71" t="str" cm="1">
         <f t="array" ref="Q120">IF(SUMPRODUCT(--(B120:E120&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -11364,7 +11361,7 @@
       </c>
       <c r="O121" s="34"/>
       <c r="P121" s="34"/>
-      <c r="Q121" s="72" t="str" cm="1">
+      <c r="Q121" s="71" t="str" cm="1">
         <f t="array" ref="Q121">IF(SUMPRODUCT(--(B121:E121&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -11428,7 +11425,7 @@
       </c>
       <c r="O122" s="34"/>
       <c r="P122" s="34"/>
-      <c r="Q122" s="72" t="str" cm="1">
+      <c r="Q122" s="71" t="str" cm="1">
         <f t="array" ref="Q122">IF(SUMPRODUCT(--(B122:E122&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -11492,7 +11489,7 @@
       </c>
       <c r="O123" s="34"/>
       <c r="P123" s="34"/>
-      <c r="Q123" s="72" t="str" cm="1">
+      <c r="Q123" s="71" t="str" cm="1">
         <f t="array" ref="Q123">IF(SUMPRODUCT(--(B123:E123&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -11556,7 +11553,7 @@
       </c>
       <c r="O124" s="34"/>
       <c r="P124" s="34"/>
-      <c r="Q124" s="72" t="str" cm="1">
+      <c r="Q124" s="71" t="str" cm="1">
         <f t="array" ref="Q124">IF(SUMPRODUCT(--(B124:E124&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -11620,7 +11617,7 @@
       </c>
       <c r="O125" s="34"/>
       <c r="P125" s="34"/>
-      <c r="Q125" s="72" t="str" cm="1">
+      <c r="Q125" s="71" t="str" cm="1">
         <f t="array" ref="Q125">IF(SUMPRODUCT(--(B125:E125&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -11684,7 +11681,7 @@
       </c>
       <c r="O126" s="34"/>
       <c r="P126" s="34"/>
-      <c r="Q126" s="72" t="str" cm="1">
+      <c r="Q126" s="71" t="str" cm="1">
         <f t="array" ref="Q126">IF(SUMPRODUCT(--(B126:E126&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -11748,7 +11745,7 @@
       </c>
       <c r="O127" s="34"/>
       <c r="P127" s="34"/>
-      <c r="Q127" s="72" t="str" cm="1">
+      <c r="Q127" s="71" t="str" cm="1">
         <f t="array" ref="Q127">IF(SUMPRODUCT(--(B127:E127&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -11812,7 +11809,7 @@
       </c>
       <c r="O128" s="34"/>
       <c r="P128" s="34"/>
-      <c r="Q128" s="72" t="str" cm="1">
+      <c r="Q128" s="71" t="str" cm="1">
         <f t="array" ref="Q128">IF(SUMPRODUCT(--(B128:E128&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -11876,7 +11873,7 @@
       </c>
       <c r="O129" s="34"/>
       <c r="P129" s="34"/>
-      <c r="Q129" s="72" t="str" cm="1">
+      <c r="Q129" s="71" t="str" cm="1">
         <f t="array" ref="Q129">IF(SUMPRODUCT(--(B129:E129&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -11940,7 +11937,7 @@
       </c>
       <c r="O130" s="34"/>
       <c r="P130" s="34"/>
-      <c r="Q130" s="72" t="str" cm="1">
+      <c r="Q130" s="71" t="str" cm="1">
         <f t="array" ref="Q130">IF(SUMPRODUCT(--(B130:E130&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -12004,7 +12001,7 @@
       </c>
       <c r="O131" s="34"/>
       <c r="P131" s="34"/>
-      <c r="Q131" s="72" t="str" cm="1">
+      <c r="Q131" s="71" t="str" cm="1">
         <f t="array" ref="Q131">IF(SUMPRODUCT(--(B131:E131&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -12068,7 +12065,7 @@
       </c>
       <c r="O132" s="34"/>
       <c r="P132" s="34"/>
-      <c r="Q132" s="72" t="str" cm="1">
+      <c r="Q132" s="71" t="str" cm="1">
         <f t="array" ref="Q132">IF(SUMPRODUCT(--(B132:E132&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -12132,7 +12129,7 @@
       </c>
       <c r="O133" s="34"/>
       <c r="P133" s="34"/>
-      <c r="Q133" s="72" t="str" cm="1">
+      <c r="Q133" s="71" t="str" cm="1">
         <f t="array" ref="Q133">IF(SUMPRODUCT(--(B133:E133&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -12196,7 +12193,7 @@
       </c>
       <c r="O134" s="34"/>
       <c r="P134" s="34"/>
-      <c r="Q134" s="72" t="str" cm="1">
+      <c r="Q134" s="71" t="str" cm="1">
         <f t="array" ref="Q134">IF(SUMPRODUCT(--(B134:E134&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -12260,7 +12257,7 @@
       </c>
       <c r="O135" s="34"/>
       <c r="P135" s="34"/>
-      <c r="Q135" s="72" t="str" cm="1">
+      <c r="Q135" s="71" t="str" cm="1">
         <f t="array" ref="Q135">IF(SUMPRODUCT(--(B135:E135&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -12324,7 +12321,7 @@
       </c>
       <c r="O136" s="34"/>
       <c r="P136" s="34"/>
-      <c r="Q136" s="72" t="str" cm="1">
+      <c r="Q136" s="71" t="str" cm="1">
         <f t="array" ref="Q136">IF(SUMPRODUCT(--(B136:E136&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -12388,7 +12385,7 @@
       </c>
       <c r="O137" s="34"/>
       <c r="P137" s="34"/>
-      <c r="Q137" s="72" t="str" cm="1">
+      <c r="Q137" s="71" t="str" cm="1">
         <f t="array" ref="Q137">IF(SUMPRODUCT(--(B137:E137&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -12452,7 +12449,7 @@
       </c>
       <c r="O138" s="34"/>
       <c r="P138" s="34"/>
-      <c r="Q138" s="72" t="str" cm="1">
+      <c r="Q138" s="71" t="str" cm="1">
         <f t="array" ref="Q138">IF(SUMPRODUCT(--(B138:E138&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -12516,7 +12513,7 @@
       </c>
       <c r="O139" s="34"/>
       <c r="P139" s="34"/>
-      <c r="Q139" s="72" t="str" cm="1">
+      <c r="Q139" s="71" t="str" cm="1">
         <f t="array" ref="Q139">IF(SUMPRODUCT(--(B139:E139&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -12580,7 +12577,7 @@
       </c>
       <c r="O140" s="34"/>
       <c r="P140" s="34"/>
-      <c r="Q140" s="72" t="str" cm="1">
+      <c r="Q140" s="71" t="str" cm="1">
         <f t="array" ref="Q140">IF(SUMPRODUCT(--(B140:E140&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -12644,7 +12641,7 @@
       </c>
       <c r="O141" s="34"/>
       <c r="P141" s="34"/>
-      <c r="Q141" s="72" t="str" cm="1">
+      <c r="Q141" s="71" t="str" cm="1">
         <f t="array" ref="Q141">IF(SUMPRODUCT(--(B141:E141&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -12708,7 +12705,7 @@
       </c>
       <c r="O142" s="34"/>
       <c r="P142" s="34"/>
-      <c r="Q142" s="72" t="str" cm="1">
+      <c r="Q142" s="71" t="str" cm="1">
         <f t="array" ref="Q142">IF(SUMPRODUCT(--(B142:E142&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -12772,7 +12769,7 @@
       </c>
       <c r="O143" s="34"/>
       <c r="P143" s="34"/>
-      <c r="Q143" s="72" t="str" cm="1">
+      <c r="Q143" s="71" t="str" cm="1">
         <f t="array" ref="Q143">IF(SUMPRODUCT(--(B143:E143&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -12836,7 +12833,7 @@
       </c>
       <c r="O144" s="34"/>
       <c r="P144" s="34"/>
-      <c r="Q144" s="72" t="str" cm="1">
+      <c r="Q144" s="71" t="str" cm="1">
         <f t="array" ref="Q144">IF(SUMPRODUCT(--(B144:E144&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -12900,7 +12897,7 @@
       </c>
       <c r="O145" s="34"/>
       <c r="P145" s="34"/>
-      <c r="Q145" s="72" t="str" cm="1">
+      <c r="Q145" s="71" t="str" cm="1">
         <f t="array" ref="Q145">IF(SUMPRODUCT(--(B145:E145&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -12964,7 +12961,7 @@
       </c>
       <c r="O146" s="34"/>
       <c r="P146" s="34"/>
-      <c r="Q146" s="72" t="str" cm="1">
+      <c r="Q146" s="71" t="str" cm="1">
         <f t="array" ref="Q146">IF(SUMPRODUCT(--(B146:E146&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -13028,7 +13025,7 @@
       </c>
       <c r="O147" s="34"/>
       <c r="P147" s="34"/>
-      <c r="Q147" s="72" t="str" cm="1">
+      <c r="Q147" s="71" t="str" cm="1">
         <f t="array" ref="Q147">IF(SUMPRODUCT(--(B147:E147&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -13092,7 +13089,7 @@
       </c>
       <c r="O148" s="34"/>
       <c r="P148" s="34"/>
-      <c r="Q148" s="72" t="str" cm="1">
+      <c r="Q148" s="71" t="str" cm="1">
         <f t="array" ref="Q148">IF(SUMPRODUCT(--(B148:E148&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -13156,7 +13153,7 @@
       </c>
       <c r="O149" s="34"/>
       <c r="P149" s="34"/>
-      <c r="Q149" s="72" t="str" cm="1">
+      <c r="Q149" s="71" t="str" cm="1">
         <f t="array" ref="Q149">IF(SUMPRODUCT(--(B149:E149&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -13220,7 +13217,7 @@
       </c>
       <c r="O150" s="34"/>
       <c r="P150" s="34"/>
-      <c r="Q150" s="72" t="str" cm="1">
+      <c r="Q150" s="71" t="str" cm="1">
         <f t="array" ref="Q150">IF(SUMPRODUCT(--(B150:E150&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -13284,7 +13281,7 @@
       </c>
       <c r="O151" s="34"/>
       <c r="P151" s="34"/>
-      <c r="Q151" s="72" t="str" cm="1">
+      <c r="Q151" s="71" t="str" cm="1">
         <f t="array" ref="Q151">IF(SUMPRODUCT(--(B151:E151&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -13348,7 +13345,7 @@
       </c>
       <c r="O152" s="34"/>
       <c r="P152" s="34"/>
-      <c r="Q152" s="72" t="str" cm="1">
+      <c r="Q152" s="71" t="str" cm="1">
         <f t="array" ref="Q152">IF(SUMPRODUCT(--(B152:E152&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -13412,7 +13409,7 @@
       </c>
       <c r="O153" s="34"/>
       <c r="P153" s="34"/>
-      <c r="Q153" s="72" t="str" cm="1">
+      <c r="Q153" s="71" t="str" cm="1">
         <f t="array" ref="Q153">IF(SUMPRODUCT(--(B153:E153&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -13476,7 +13473,7 @@
       </c>
       <c r="O154" s="34"/>
       <c r="P154" s="34"/>
-      <c r="Q154" s="72" t="str" cm="1">
+      <c r="Q154" s="71" t="str" cm="1">
         <f t="array" ref="Q154">IF(SUMPRODUCT(--(B154:E154&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -13540,7 +13537,7 @@
       </c>
       <c r="O155" s="34"/>
       <c r="P155" s="34"/>
-      <c r="Q155" s="72" t="str" cm="1">
+      <c r="Q155" s="71" t="str" cm="1">
         <f t="array" ref="Q155">IF(SUMPRODUCT(--(B155:E155&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -13604,7 +13601,7 @@
       </c>
       <c r="O156" s="34"/>
       <c r="P156" s="34"/>
-      <c r="Q156" s="72" t="str" cm="1">
+      <c r="Q156" s="71" t="str" cm="1">
         <f t="array" ref="Q156">IF(SUMPRODUCT(--(B156:E156&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -13668,7 +13665,7 @@
       </c>
       <c r="O157" s="34"/>
       <c r="P157" s="34"/>
-      <c r="Q157" s="72" t="str" cm="1">
+      <c r="Q157" s="71" t="str" cm="1">
         <f t="array" ref="Q157">IF(SUMPRODUCT(--(B157:E157&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -13732,7 +13729,7 @@
       </c>
       <c r="O158" s="34"/>
       <c r="P158" s="34"/>
-      <c r="Q158" s="72" t="str" cm="1">
+      <c r="Q158" s="71" t="str" cm="1">
         <f t="array" ref="Q158">IF(SUMPRODUCT(--(B158:E158&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -13796,7 +13793,7 @@
       </c>
       <c r="O159" s="34"/>
       <c r="P159" s="34"/>
-      <c r="Q159" s="72" t="str" cm="1">
+      <c r="Q159" s="71" t="str" cm="1">
         <f t="array" ref="Q159">IF(SUMPRODUCT(--(B159:E159&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -13860,7 +13857,7 @@
       </c>
       <c r="O160" s="34"/>
       <c r="P160" s="34"/>
-      <c r="Q160" s="72" t="str" cm="1">
+      <c r="Q160" s="71" t="str" cm="1">
         <f t="array" ref="Q160">IF(SUMPRODUCT(--(B160:E160&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -13924,7 +13921,7 @@
       </c>
       <c r="O161" s="34"/>
       <c r="P161" s="34"/>
-      <c r="Q161" s="72" t="str" cm="1">
+      <c r="Q161" s="71" t="str" cm="1">
         <f t="array" ref="Q161">IF(SUMPRODUCT(--(B161:E161&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -13988,7 +13985,7 @@
       </c>
       <c r="O162" s="34"/>
       <c r="P162" s="34"/>
-      <c r="Q162" s="72" t="str" cm="1">
+      <c r="Q162" s="71" t="str" cm="1">
         <f t="array" ref="Q162">IF(SUMPRODUCT(--(B162:E162&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -14052,7 +14049,7 @@
       </c>
       <c r="O163" s="34"/>
       <c r="P163" s="34"/>
-      <c r="Q163" s="72" t="str" cm="1">
+      <c r="Q163" s="71" t="str" cm="1">
         <f t="array" ref="Q163">IF(SUMPRODUCT(--(B163:E163&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -14116,7 +14113,7 @@
       </c>
       <c r="O164" s="34"/>
       <c r="P164" s="34"/>
-      <c r="Q164" s="72" t="str" cm="1">
+      <c r="Q164" s="71" t="str" cm="1">
         <f t="array" ref="Q164">IF(SUMPRODUCT(--(B164:E164&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -14180,7 +14177,7 @@
       </c>
       <c r="O165" s="34"/>
       <c r="P165" s="34"/>
-      <c r="Q165" s="72" t="str" cm="1">
+      <c r="Q165" s="71" t="str" cm="1">
         <f t="array" ref="Q165">IF(SUMPRODUCT(--(B165:E165&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -14244,7 +14241,7 @@
       </c>
       <c r="O166" s="34"/>
       <c r="P166" s="34"/>
-      <c r="Q166" s="72" t="str" cm="1">
+      <c r="Q166" s="71" t="str" cm="1">
         <f t="array" ref="Q166">IF(SUMPRODUCT(--(B166:E166&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -14308,7 +14305,7 @@
       </c>
       <c r="O167" s="34"/>
       <c r="P167" s="34"/>
-      <c r="Q167" s="72" t="str" cm="1">
+      <c r="Q167" s="71" t="str" cm="1">
         <f t="array" ref="Q167">IF(SUMPRODUCT(--(B167:E167&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -14372,7 +14369,7 @@
       </c>
       <c r="O168" s="34"/>
       <c r="P168" s="34"/>
-      <c r="Q168" s="72" t="str" cm="1">
+      <c r="Q168" s="71" t="str" cm="1">
         <f t="array" ref="Q168">IF(SUMPRODUCT(--(B168:E168&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -14436,7 +14433,7 @@
       </c>
       <c r="O169" s="34"/>
       <c r="P169" s="34"/>
-      <c r="Q169" s="72" t="str" cm="1">
+      <c r="Q169" s="71" t="str" cm="1">
         <f t="array" ref="Q169">IF(SUMPRODUCT(--(B169:E169&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -14500,7 +14497,7 @@
       </c>
       <c r="O170" s="34"/>
       <c r="P170" s="34"/>
-      <c r="Q170" s="72" t="str" cm="1">
+      <c r="Q170" s="71" t="str" cm="1">
         <f t="array" ref="Q170">IF(SUMPRODUCT(--(B170:E170&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -14564,7 +14561,7 @@
       </c>
       <c r="O171" s="34"/>
       <c r="P171" s="34"/>
-      <c r="Q171" s="72" t="str" cm="1">
+      <c r="Q171" s="71" t="str" cm="1">
         <f t="array" ref="Q171">IF(SUMPRODUCT(--(B171:E171&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -14628,7 +14625,7 @@
       </c>
       <c r="O172" s="34"/>
       <c r="P172" s="34"/>
-      <c r="Q172" s="72" t="str" cm="1">
+      <c r="Q172" s="71" t="str" cm="1">
         <f t="array" ref="Q172">IF(SUMPRODUCT(--(B172:E172&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -14692,7 +14689,7 @@
       </c>
       <c r="O173" s="34"/>
       <c r="P173" s="34"/>
-      <c r="Q173" s="72" t="str" cm="1">
+      <c r="Q173" s="71" t="str" cm="1">
         <f t="array" ref="Q173">IF(SUMPRODUCT(--(B173:E173&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -14756,7 +14753,7 @@
       </c>
       <c r="O174" s="34"/>
       <c r="P174" s="34"/>
-      <c r="Q174" s="72" t="str" cm="1">
+      <c r="Q174" s="71" t="str" cm="1">
         <f t="array" ref="Q174">IF(SUMPRODUCT(--(B174:E174&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -14820,7 +14817,7 @@
       </c>
       <c r="O175" s="34"/>
       <c r="P175" s="34"/>
-      <c r="Q175" s="72" t="str" cm="1">
+      <c r="Q175" s="71" t="str" cm="1">
         <f t="array" ref="Q175">IF(SUMPRODUCT(--(B175:E175&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -14884,7 +14881,7 @@
       </c>
       <c r="O176" s="34"/>
       <c r="P176" s="34"/>
-      <c r="Q176" s="72" t="str" cm="1">
+      <c r="Q176" s="71" t="str" cm="1">
         <f t="array" ref="Q176">IF(SUMPRODUCT(--(B176:E176&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -14948,7 +14945,7 @@
       </c>
       <c r="O177" s="34"/>
       <c r="P177" s="34"/>
-      <c r="Q177" s="72" t="str" cm="1">
+      <c r="Q177" s="71" t="str" cm="1">
         <f t="array" ref="Q177">IF(SUMPRODUCT(--(B177:E177&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -15012,7 +15009,7 @@
       </c>
       <c r="O178" s="34"/>
       <c r="P178" s="34"/>
-      <c r="Q178" s="72" t="str" cm="1">
+      <c r="Q178" s="71" t="str" cm="1">
         <f t="array" ref="Q178">IF(SUMPRODUCT(--(B178:E178&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -15076,7 +15073,7 @@
       </c>
       <c r="O179" s="34"/>
       <c r="P179" s="34"/>
-      <c r="Q179" s="72" t="str" cm="1">
+      <c r="Q179" s="71" t="str" cm="1">
         <f t="array" ref="Q179">IF(SUMPRODUCT(--(B179:E179&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -15140,7 +15137,7 @@
       </c>
       <c r="O180" s="34"/>
       <c r="P180" s="34"/>
-      <c r="Q180" s="72" t="str" cm="1">
+      <c r="Q180" s="71" t="str" cm="1">
         <f t="array" ref="Q180">IF(SUMPRODUCT(--(B180:E180&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -15204,7 +15201,7 @@
       </c>
       <c r="O181" s="34"/>
       <c r="P181" s="34"/>
-      <c r="Q181" s="72" t="str" cm="1">
+      <c r="Q181" s="71" t="str" cm="1">
         <f t="array" ref="Q181">IF(SUMPRODUCT(--(B181:E181&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -15268,7 +15265,7 @@
       </c>
       <c r="O182" s="34"/>
       <c r="P182" s="34"/>
-      <c r="Q182" s="72" t="str" cm="1">
+      <c r="Q182" s="71" t="str" cm="1">
         <f t="array" ref="Q182">IF(SUMPRODUCT(--(B182:E182&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -15332,7 +15329,7 @@
       </c>
       <c r="O183" s="34"/>
       <c r="P183" s="34"/>
-      <c r="Q183" s="72" t="str" cm="1">
+      <c r="Q183" s="71" t="str" cm="1">
         <f t="array" ref="Q183">IF(SUMPRODUCT(--(B183:E183&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -15396,7 +15393,7 @@
       </c>
       <c r="O184" s="34"/>
       <c r="P184" s="34"/>
-      <c r="Q184" s="72" t="str" cm="1">
+      <c r="Q184" s="71" t="str" cm="1">
         <f t="array" ref="Q184">IF(SUMPRODUCT(--(B184:E184&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -15460,7 +15457,7 @@
       </c>
       <c r="O185" s="34"/>
       <c r="P185" s="34"/>
-      <c r="Q185" s="72" t="str" cm="1">
+      <c r="Q185" s="71" t="str" cm="1">
         <f t="array" ref="Q185">IF(SUMPRODUCT(--(B185:E185&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -15524,7 +15521,7 @@
       </c>
       <c r="O186" s="34"/>
       <c r="P186" s="34"/>
-      <c r="Q186" s="72" t="str" cm="1">
+      <c r="Q186" s="71" t="str" cm="1">
         <f t="array" ref="Q186">IF(SUMPRODUCT(--(B186:E186&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -15588,7 +15585,7 @@
       </c>
       <c r="O187" s="34"/>
       <c r="P187" s="34"/>
-      <c r="Q187" s="72" t="str" cm="1">
+      <c r="Q187" s="71" t="str" cm="1">
         <f t="array" ref="Q187">IF(SUMPRODUCT(--(B187:E187&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -15652,7 +15649,7 @@
       </c>
       <c r="O188" s="34"/>
       <c r="P188" s="34"/>
-      <c r="Q188" s="72" t="str" cm="1">
+      <c r="Q188" s="71" t="str" cm="1">
         <f t="array" ref="Q188">IF(SUMPRODUCT(--(B188:E188&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -15716,7 +15713,7 @@
       </c>
       <c r="O189" s="34"/>
       <c r="P189" s="34"/>
-      <c r="Q189" s="72" t="str" cm="1">
+      <c r="Q189" s="71" t="str" cm="1">
         <f t="array" ref="Q189">IF(SUMPRODUCT(--(B189:E189&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -15780,7 +15777,7 @@
       </c>
       <c r="O190" s="34"/>
       <c r="P190" s="34"/>
-      <c r="Q190" s="72" t="str" cm="1">
+      <c r="Q190" s="71" t="str" cm="1">
         <f t="array" ref="Q190">IF(SUMPRODUCT(--(B190:E190&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -15844,7 +15841,7 @@
       </c>
       <c r="O191" s="34"/>
       <c r="P191" s="34"/>
-      <c r="Q191" s="72" t="str" cm="1">
+      <c r="Q191" s="71" t="str" cm="1">
         <f t="array" ref="Q191">IF(SUMPRODUCT(--(B191:E191&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -15908,7 +15905,7 @@
       </c>
       <c r="O192" s="34"/>
       <c r="P192" s="34"/>
-      <c r="Q192" s="72" t="str" cm="1">
+      <c r="Q192" s="71" t="str" cm="1">
         <f t="array" ref="Q192">IF(SUMPRODUCT(--(B192:E192&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -15972,7 +15969,7 @@
       </c>
       <c r="O193" s="34"/>
       <c r="P193" s="34"/>
-      <c r="Q193" s="72" t="str" cm="1">
+      <c r="Q193" s="71" t="str" cm="1">
         <f t="array" ref="Q193">IF(SUMPRODUCT(--(B193:E193&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -16036,7 +16033,7 @@
       </c>
       <c r="O194" s="34"/>
       <c r="P194" s="34"/>
-      <c r="Q194" s="72" t="str" cm="1">
+      <c r="Q194" s="71" t="str" cm="1">
         <f t="array" ref="Q194">IF(SUMPRODUCT(--(B194:E194&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -16100,7 +16097,7 @@
       </c>
       <c r="O195" s="34"/>
       <c r="P195" s="34"/>
-      <c r="Q195" s="72" t="str" cm="1">
+      <c r="Q195" s="71" t="str" cm="1">
         <f t="array" ref="Q195">IF(SUMPRODUCT(--(B195:E195&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -16164,7 +16161,7 @@
       </c>
       <c r="O196" s="34"/>
       <c r="P196" s="34"/>
-      <c r="Q196" s="72" t="str" cm="1">
+      <c r="Q196" s="71" t="str" cm="1">
         <f t="array" ref="Q196">IF(SUMPRODUCT(--(B196:E196&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -16228,7 +16225,7 @@
       </c>
       <c r="O197" s="34"/>
       <c r="P197" s="34"/>
-      <c r="Q197" s="72" t="str" cm="1">
+      <c r="Q197" s="71" t="str" cm="1">
         <f t="array" ref="Q197">IF(SUMPRODUCT(--(B197:E197&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -16292,7 +16289,7 @@
       </c>
       <c r="O198" s="34"/>
       <c r="P198" s="34"/>
-      <c r="Q198" s="72" t="str" cm="1">
+      <c r="Q198" s="71" t="str" cm="1">
         <f t="array" ref="Q198">IF(SUMPRODUCT(--(B198:E198&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -16356,7 +16353,7 @@
       </c>
       <c r="O199" s="34"/>
       <c r="P199" s="34"/>
-      <c r="Q199" s="72" t="str" cm="1">
+      <c r="Q199" s="71" t="str" cm="1">
         <f t="array" ref="Q199">IF(SUMPRODUCT(--(B199:E199&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -16420,7 +16417,7 @@
       </c>
       <c r="O200" s="34"/>
       <c r="P200" s="34"/>
-      <c r="Q200" s="72" t="str" cm="1">
+      <c r="Q200" s="71" t="str" cm="1">
         <f t="array" ref="Q200">IF(SUMPRODUCT(--(B200:E200&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -16484,7 +16481,7 @@
       </c>
       <c r="O201" s="34"/>
       <c r="P201" s="34"/>
-      <c r="Q201" s="72" t="str" cm="1">
+      <c r="Q201" s="71" t="str" cm="1">
         <f t="array" ref="Q201">IF(SUMPRODUCT(--(B201:E201&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -16548,7 +16545,7 @@
       </c>
       <c r="O202" s="34"/>
       <c r="P202" s="34"/>
-      <c r="Q202" s="72" t="str" cm="1">
+      <c r="Q202" s="71" t="str" cm="1">
         <f t="array" ref="Q202">IF(SUMPRODUCT(--(B202:E202&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -16612,7 +16609,7 @@
       </c>
       <c r="O203" s="34"/>
       <c r="P203" s="34"/>
-      <c r="Q203" s="72" t="str" cm="1">
+      <c r="Q203" s="71" t="str" cm="1">
         <f t="array" ref="Q203">IF(SUMPRODUCT(--(B203:E203&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -16676,7 +16673,7 @@
       </c>
       <c r="O204" s="34"/>
       <c r="P204" s="34"/>
-      <c r="Q204" s="72" t="str" cm="1">
+      <c r="Q204" s="71" t="str" cm="1">
         <f t="array" ref="Q204">IF(SUMPRODUCT(--(B204:E204&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -16740,7 +16737,7 @@
       </c>
       <c r="O205" s="34"/>
       <c r="P205" s="34"/>
-      <c r="Q205" s="72" t="str" cm="1">
+      <c r="Q205" s="71" t="str" cm="1">
         <f t="array" ref="Q205">IF(SUMPRODUCT(--(B205:E205&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -16804,7 +16801,7 @@
       </c>
       <c r="O206" s="34"/>
       <c r="P206" s="34"/>
-      <c r="Q206" s="72" t="str" cm="1">
+      <c r="Q206" s="71" t="str" cm="1">
         <f t="array" ref="Q206">IF(SUMPRODUCT(--(B206:E206&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -16868,7 +16865,7 @@
       </c>
       <c r="O207" s="34"/>
       <c r="P207" s="34"/>
-      <c r="Q207" s="72" t="str" cm="1">
+      <c r="Q207" s="71" t="str" cm="1">
         <f t="array" ref="Q207">IF(SUMPRODUCT(--(B207:E207&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -16932,7 +16929,7 @@
       </c>
       <c r="O208" s="34"/>
       <c r="P208" s="34"/>
-      <c r="Q208" s="72" t="str" cm="1">
+      <c r="Q208" s="71" t="str" cm="1">
         <f t="array" ref="Q208">IF(SUMPRODUCT(--(B208:E208&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -16996,7 +16993,7 @@
       </c>
       <c r="O209" s="34"/>
       <c r="P209" s="34"/>
-      <c r="Q209" s="72" t="str" cm="1">
+      <c r="Q209" s="71" t="str" cm="1">
         <f t="array" ref="Q209">IF(SUMPRODUCT(--(B209:E209&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -17060,7 +17057,7 @@
       </c>
       <c r="O210" s="34"/>
       <c r="P210" s="34"/>
-      <c r="Q210" s="72" t="str" cm="1">
+      <c r="Q210" s="71" t="str" cm="1">
         <f t="array" ref="Q210">IF(SUMPRODUCT(--(B210:E210&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -17124,7 +17121,7 @@
       </c>
       <c r="O211" s="34"/>
       <c r="P211" s="34"/>
-      <c r="Q211" s="72" t="str" cm="1">
+      <c r="Q211" s="71" t="str" cm="1">
         <f t="array" ref="Q211">IF(SUMPRODUCT(--(B211:E211&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -17188,7 +17185,7 @@
       </c>
       <c r="O212" s="34"/>
       <c r="P212" s="34"/>
-      <c r="Q212" s="72" t="str" cm="1">
+      <c r="Q212" s="71" t="str" cm="1">
         <f t="array" ref="Q212">IF(SUMPRODUCT(--(B212:E212&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -17252,7 +17249,7 @@
       </c>
       <c r="O213" s="34"/>
       <c r="P213" s="34"/>
-      <c r="Q213" s="72" t="str" cm="1">
+      <c r="Q213" s="71" t="str" cm="1">
         <f t="array" ref="Q213">IF(SUMPRODUCT(--(B213:E213&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -17316,7 +17313,7 @@
       </c>
       <c r="O214" s="34"/>
       <c r="P214" s="34"/>
-      <c r="Q214" s="72" t="str" cm="1">
+      <c r="Q214" s="71" t="str" cm="1">
         <f t="array" ref="Q214">IF(SUMPRODUCT(--(B214:E214&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -17380,7 +17377,7 @@
       </c>
       <c r="O215" s="34"/>
       <c r="P215" s="34"/>
-      <c r="Q215" s="72" t="str" cm="1">
+      <c r="Q215" s="71" t="str" cm="1">
         <f t="array" ref="Q215">IF(SUMPRODUCT(--(B215:E215&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -17444,7 +17441,7 @@
       </c>
       <c r="O216" s="34"/>
       <c r="P216" s="34"/>
-      <c r="Q216" s="72" t="str" cm="1">
+      <c r="Q216" s="71" t="str" cm="1">
         <f t="array" ref="Q216">IF(SUMPRODUCT(--(B216:E216&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -17508,7 +17505,7 @@
       </c>
       <c r="O217" s="34"/>
       <c r="P217" s="34"/>
-      <c r="Q217" s="72" t="str" cm="1">
+      <c r="Q217" s="71" t="str" cm="1">
         <f t="array" ref="Q217">IF(SUMPRODUCT(--(B217:E217&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -17572,7 +17569,7 @@
       </c>
       <c r="O218" s="34"/>
       <c r="P218" s="34"/>
-      <c r="Q218" s="72" t="str" cm="1">
+      <c r="Q218" s="71" t="str" cm="1">
         <f t="array" ref="Q218">IF(SUMPRODUCT(--(B218:E218&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -17636,7 +17633,7 @@
       </c>
       <c r="O219" s="34"/>
       <c r="P219" s="34"/>
-      <c r="Q219" s="72" t="str" cm="1">
+      <c r="Q219" s="71" t="str" cm="1">
         <f t="array" ref="Q219">IF(SUMPRODUCT(--(B219:E219&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -17700,7 +17697,7 @@
       </c>
       <c r="O220" s="34"/>
       <c r="P220" s="34"/>
-      <c r="Q220" s="72" t="str" cm="1">
+      <c r="Q220" s="71" t="str" cm="1">
         <f t="array" ref="Q220">IF(SUMPRODUCT(--(B220:E220&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -17764,7 +17761,7 @@
       </c>
       <c r="O221" s="34"/>
       <c r="P221" s="34"/>
-      <c r="Q221" s="72" t="str" cm="1">
+      <c r="Q221" s="71" t="str" cm="1">
         <f t="array" ref="Q221">IF(SUMPRODUCT(--(B221:E221&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -17828,7 +17825,7 @@
       </c>
       <c r="O222" s="34"/>
       <c r="P222" s="34"/>
-      <c r="Q222" s="72" t="str" cm="1">
+      <c r="Q222" s="71" t="str" cm="1">
         <f t="array" ref="Q222">IF(SUMPRODUCT(--(B222:E222&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -17892,7 +17889,7 @@
       </c>
       <c r="O223" s="34"/>
       <c r="P223" s="34"/>
-      <c r="Q223" s="72" t="str" cm="1">
+      <c r="Q223" s="71" t="str" cm="1">
         <f t="array" ref="Q223">IF(SUMPRODUCT(--(B223:E223&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -17956,7 +17953,7 @@
       </c>
       <c r="O224" s="34"/>
       <c r="P224" s="34"/>
-      <c r="Q224" s="72" t="str" cm="1">
+      <c r="Q224" s="71" t="str" cm="1">
         <f t="array" ref="Q224">IF(SUMPRODUCT(--(B224:E224&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -18020,7 +18017,7 @@
       </c>
       <c r="O225" s="34"/>
       <c r="P225" s="34"/>
-      <c r="Q225" s="72" t="str" cm="1">
+      <c r="Q225" s="71" t="str" cm="1">
         <f t="array" ref="Q225">IF(SUMPRODUCT(--(B225:E225&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -18084,7 +18081,7 @@
       </c>
       <c r="O226" s="34"/>
       <c r="P226" s="34"/>
-      <c r="Q226" s="72" t="str" cm="1">
+      <c r="Q226" s="71" t="str" cm="1">
         <f t="array" ref="Q226">IF(SUMPRODUCT(--(B226:E226&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -18148,7 +18145,7 @@
       </c>
       <c r="O227" s="34"/>
       <c r="P227" s="34"/>
-      <c r="Q227" s="72" t="str" cm="1">
+      <c r="Q227" s="71" t="str" cm="1">
         <f t="array" ref="Q227">IF(SUMPRODUCT(--(B227:E227&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -18212,7 +18209,7 @@
       </c>
       <c r="O228" s="34"/>
       <c r="P228" s="34"/>
-      <c r="Q228" s="72" t="str" cm="1">
+      <c r="Q228" s="71" t="str" cm="1">
         <f t="array" ref="Q228">IF(SUMPRODUCT(--(B228:E228&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -18276,7 +18273,7 @@
       </c>
       <c r="O229" s="34"/>
       <c r="P229" s="34"/>
-      <c r="Q229" s="72" t="str" cm="1">
+      <c r="Q229" s="71" t="str" cm="1">
         <f t="array" ref="Q229">IF(SUMPRODUCT(--(B229:E229&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -18340,7 +18337,7 @@
       </c>
       <c r="O230" s="34"/>
       <c r="P230" s="34"/>
-      <c r="Q230" s="72" t="str" cm="1">
+      <c r="Q230" s="71" t="str" cm="1">
         <f t="array" ref="Q230">IF(SUMPRODUCT(--(B230:E230&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -18404,7 +18401,7 @@
       </c>
       <c r="O231" s="34"/>
       <c r="P231" s="34"/>
-      <c r="Q231" s="72" t="str" cm="1">
+      <c r="Q231" s="71" t="str" cm="1">
         <f t="array" ref="Q231">IF(SUMPRODUCT(--(B231:E231&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -18468,7 +18465,7 @@
       </c>
       <c r="O232" s="34"/>
       <c r="P232" s="34"/>
-      <c r="Q232" s="72" t="str" cm="1">
+      <c r="Q232" s="71" t="str" cm="1">
         <f t="array" ref="Q232">IF(SUMPRODUCT(--(B232:E232&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -18532,7 +18529,7 @@
       </c>
       <c r="O233" s="34"/>
       <c r="P233" s="34"/>
-      <c r="Q233" s="72" t="str" cm="1">
+      <c r="Q233" s="71" t="str" cm="1">
         <f t="array" ref="Q233">IF(SUMPRODUCT(--(B233:E233&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -18596,7 +18593,7 @@
       </c>
       <c r="O234" s="34"/>
       <c r="P234" s="34"/>
-      <c r="Q234" s="72" t="str" cm="1">
+      <c r="Q234" s="71" t="str" cm="1">
         <f t="array" ref="Q234">IF(SUMPRODUCT(--(B234:E234&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -18660,7 +18657,7 @@
       </c>
       <c r="O235" s="34"/>
       <c r="P235" s="34"/>
-      <c r="Q235" s="72" t="str" cm="1">
+      <c r="Q235" s="71" t="str" cm="1">
         <f t="array" ref="Q235">IF(SUMPRODUCT(--(B235:E235&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -18724,7 +18721,7 @@
       </c>
       <c r="O236" s="34"/>
       <c r="P236" s="34"/>
-      <c r="Q236" s="72" t="str" cm="1">
+      <c r="Q236" s="71" t="str" cm="1">
         <f t="array" ref="Q236">IF(SUMPRODUCT(--(B236:E236&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -18788,7 +18785,7 @@
       </c>
       <c r="O237" s="34"/>
       <c r="P237" s="34"/>
-      <c r="Q237" s="72" t="str" cm="1">
+      <c r="Q237" s="71" t="str" cm="1">
         <f t="array" ref="Q237">IF(SUMPRODUCT(--(B237:E237&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -18852,7 +18849,7 @@
       </c>
       <c r="O238" s="34"/>
       <c r="P238" s="34"/>
-      <c r="Q238" s="72" t="str" cm="1">
+      <c r="Q238" s="71" t="str" cm="1">
         <f t="array" ref="Q238">IF(SUMPRODUCT(--(B238:E238&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -18916,7 +18913,7 @@
       </c>
       <c r="O239" s="34"/>
       <c r="P239" s="34"/>
-      <c r="Q239" s="72" t="str" cm="1">
+      <c r="Q239" s="71" t="str" cm="1">
         <f t="array" ref="Q239">IF(SUMPRODUCT(--(B239:E239&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -18980,7 +18977,7 @@
       </c>
       <c r="O240" s="34"/>
       <c r="P240" s="34"/>
-      <c r="Q240" s="72" t="str" cm="1">
+      <c r="Q240" s="71" t="str" cm="1">
         <f t="array" ref="Q240">IF(SUMPRODUCT(--(B240:E240&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -19044,7 +19041,7 @@
       </c>
       <c r="O241" s="34"/>
       <c r="P241" s="34"/>
-      <c r="Q241" s="72" t="str" cm="1">
+      <c r="Q241" s="71" t="str" cm="1">
         <f t="array" ref="Q241">IF(SUMPRODUCT(--(B241:E241&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -19108,7 +19105,7 @@
       </c>
       <c r="O242" s="34"/>
       <c r="P242" s="34"/>
-      <c r="Q242" s="72" t="str" cm="1">
+      <c r="Q242" s="71" t="str" cm="1">
         <f t="array" ref="Q242">IF(SUMPRODUCT(--(B242:E242&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -19172,7 +19169,7 @@
       </c>
       <c r="O243" s="34"/>
       <c r="P243" s="34"/>
-      <c r="Q243" s="72" t="str" cm="1">
+      <c r="Q243" s="71" t="str" cm="1">
         <f t="array" ref="Q243">IF(SUMPRODUCT(--(B243:E243&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -19236,7 +19233,7 @@
       </c>
       <c r="O244" s="34"/>
       <c r="P244" s="34"/>
-      <c r="Q244" s="72" t="str" cm="1">
+      <c r="Q244" s="71" t="str" cm="1">
         <f t="array" ref="Q244">IF(SUMPRODUCT(--(B244:E244&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -19300,7 +19297,7 @@
       </c>
       <c r="O245" s="34"/>
       <c r="P245" s="34"/>
-      <c r="Q245" s="72" t="str" cm="1">
+      <c r="Q245" s="71" t="str" cm="1">
         <f t="array" ref="Q245">IF(SUMPRODUCT(--(B245:E245&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -19364,7 +19361,7 @@
       </c>
       <c r="O246" s="34"/>
       <c r="P246" s="34"/>
-      <c r="Q246" s="72" t="str" cm="1">
+      <c r="Q246" s="71" t="str" cm="1">
         <f t="array" ref="Q246">IF(SUMPRODUCT(--(B246:E246&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -19428,7 +19425,7 @@
       </c>
       <c r="O247" s="34"/>
       <c r="P247" s="34"/>
-      <c r="Q247" s="72" t="str" cm="1">
+      <c r="Q247" s="71" t="str" cm="1">
         <f t="array" ref="Q247">IF(SUMPRODUCT(--(B247:E247&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -19492,7 +19489,7 @@
       </c>
       <c r="O248" s="34"/>
       <c r="P248" s="34"/>
-      <c r="Q248" s="72" t="str" cm="1">
+      <c r="Q248" s="71" t="str" cm="1">
         <f t="array" ref="Q248">IF(SUMPRODUCT(--(B248:E248&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -19556,7 +19553,7 @@
       </c>
       <c r="O249" s="34"/>
       <c r="P249" s="34"/>
-      <c r="Q249" s="72" t="str" cm="1">
+      <c r="Q249" s="71" t="str" cm="1">
         <f t="array" ref="Q249">IF(SUMPRODUCT(--(B249:E249&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -19620,7 +19617,7 @@
       </c>
       <c r="O250" s="34"/>
       <c r="P250" s="34"/>
-      <c r="Q250" s="72" t="str" cm="1">
+      <c r="Q250" s="71" t="str" cm="1">
         <f t="array" ref="Q250">IF(SUMPRODUCT(--(B250:E250&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -19684,7 +19681,7 @@
       </c>
       <c r="O251" s="34"/>
       <c r="P251" s="34"/>
-      <c r="Q251" s="72" t="str" cm="1">
+      <c r="Q251" s="71" t="str" cm="1">
         <f t="array" ref="Q251">IF(SUMPRODUCT(--(B251:E251&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -19748,7 +19745,7 @@
       </c>
       <c r="O252" s="34"/>
       <c r="P252" s="34"/>
-      <c r="Q252" s="72" t="str" cm="1">
+      <c r="Q252" s="71" t="str" cm="1">
         <f t="array" ref="Q252">IF(SUMPRODUCT(--(B252:E252&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -19812,7 +19809,7 @@
       </c>
       <c r="O253" s="34"/>
       <c r="P253" s="34"/>
-      <c r="Q253" s="72" t="str" cm="1">
+      <c r="Q253" s="71" t="str" cm="1">
         <f t="array" ref="Q253">IF(SUMPRODUCT(--(B253:E253&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -19876,7 +19873,7 @@
       </c>
       <c r="O254" s="34"/>
       <c r="P254" s="34"/>
-      <c r="Q254" s="72" t="str" cm="1">
+      <c r="Q254" s="71" t="str" cm="1">
         <f t="array" ref="Q254">IF(SUMPRODUCT(--(B254:E254&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -19940,7 +19937,7 @@
       </c>
       <c r="O255" s="34"/>
       <c r="P255" s="34"/>
-      <c r="Q255" s="72" t="str" cm="1">
+      <c r="Q255" s="71" t="str" cm="1">
         <f t="array" ref="Q255">IF(SUMPRODUCT(--(B255:E255&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -20004,7 +20001,7 @@
       </c>
       <c r="O256" s="34"/>
       <c r="P256" s="34"/>
-      <c r="Q256" s="72" t="str" cm="1">
+      <c r="Q256" s="71" t="str" cm="1">
         <f t="array" ref="Q256">IF(SUMPRODUCT(--(B256:E256&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -20068,7 +20065,7 @@
       </c>
       <c r="O257" s="34"/>
       <c r="P257" s="34"/>
-      <c r="Q257" s="72" t="str" cm="1">
+      <c r="Q257" s="71" t="str" cm="1">
         <f t="array" ref="Q257">IF(SUMPRODUCT(--(B257:E257&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -20132,7 +20129,7 @@
       </c>
       <c r="O258" s="34"/>
       <c r="P258" s="34"/>
-      <c r="Q258" s="72" t="str" cm="1">
+      <c r="Q258" s="71" t="str" cm="1">
         <f t="array" ref="Q258">IF(SUMPRODUCT(--(B258:E258&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -20196,7 +20193,7 @@
       </c>
       <c r="O259" s="34"/>
       <c r="P259" s="34"/>
-      <c r="Q259" s="72" t="str" cm="1">
+      <c r="Q259" s="71" t="str" cm="1">
         <f t="array" ref="Q259">IF(SUMPRODUCT(--(B259:E259&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -20260,7 +20257,7 @@
       </c>
       <c r="O260" s="34"/>
       <c r="P260" s="34"/>
-      <c r="Q260" s="72" t="str" cm="1">
+      <c r="Q260" s="71" t="str" cm="1">
         <f t="array" ref="Q260">IF(SUMPRODUCT(--(B260:E260&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -20324,7 +20321,7 @@
       </c>
       <c r="O261" s="34"/>
       <c r="P261" s="34"/>
-      <c r="Q261" s="72" t="str" cm="1">
+      <c r="Q261" s="71" t="str" cm="1">
         <f t="array" ref="Q261">IF(SUMPRODUCT(--(B261:E261&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -20388,7 +20385,7 @@
       </c>
       <c r="O262" s="34"/>
       <c r="P262" s="34"/>
-      <c r="Q262" s="72" t="str" cm="1">
+      <c r="Q262" s="71" t="str" cm="1">
         <f t="array" ref="Q262">IF(SUMPRODUCT(--(B262:E262&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -20452,7 +20449,7 @@
       </c>
       <c r="O263" s="34"/>
       <c r="P263" s="34"/>
-      <c r="Q263" s="72" t="str" cm="1">
+      <c r="Q263" s="71" t="str" cm="1">
         <f t="array" ref="Q263">IF(SUMPRODUCT(--(B263:E263&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -20516,7 +20513,7 @@
       </c>
       <c r="O264" s="34"/>
       <c r="P264" s="34"/>
-      <c r="Q264" s="72" t="str" cm="1">
+      <c r="Q264" s="71" t="str" cm="1">
         <f t="array" ref="Q264">IF(SUMPRODUCT(--(B264:E264&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -20580,7 +20577,7 @@
       </c>
       <c r="O265" s="34"/>
       <c r="P265" s="34"/>
-      <c r="Q265" s="72" t="str" cm="1">
+      <c r="Q265" s="71" t="str" cm="1">
         <f t="array" ref="Q265">IF(SUMPRODUCT(--(B265:E265&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -20644,7 +20641,7 @@
       </c>
       <c r="O266" s="34"/>
       <c r="P266" s="34"/>
-      <c r="Q266" s="72" t="str" cm="1">
+      <c r="Q266" s="71" t="str" cm="1">
         <f t="array" ref="Q266">IF(SUMPRODUCT(--(B266:E266&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -20708,7 +20705,7 @@
       </c>
       <c r="O267" s="34"/>
       <c r="P267" s="34"/>
-      <c r="Q267" s="72" t="str" cm="1">
+      <c r="Q267" s="71" t="str" cm="1">
         <f t="array" ref="Q267">IF(SUMPRODUCT(--(B267:E267&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -20772,7 +20769,7 @@
       </c>
       <c r="O268" s="34"/>
       <c r="P268" s="34"/>
-      <c r="Q268" s="72" t="str" cm="1">
+      <c r="Q268" s="71" t="str" cm="1">
         <f t="array" ref="Q268">IF(SUMPRODUCT(--(B268:E268&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -20836,7 +20833,7 @@
       </c>
       <c r="O269" s="34"/>
       <c r="P269" s="34"/>
-      <c r="Q269" s="72" t="str" cm="1">
+      <c r="Q269" s="71" t="str" cm="1">
         <f t="array" ref="Q269">IF(SUMPRODUCT(--(B269:E269&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -20900,7 +20897,7 @@
       </c>
       <c r="O270" s="34"/>
       <c r="P270" s="34"/>
-      <c r="Q270" s="72" t="str" cm="1">
+      <c r="Q270" s="71" t="str" cm="1">
         <f t="array" ref="Q270">IF(SUMPRODUCT(--(B270:E270&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -20964,7 +20961,7 @@
       </c>
       <c r="O271" s="34"/>
       <c r="P271" s="34"/>
-      <c r="Q271" s="72" t="str" cm="1">
+      <c r="Q271" s="71" t="str" cm="1">
         <f t="array" ref="Q271">IF(SUMPRODUCT(--(B271:E271&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -21028,7 +21025,7 @@
       </c>
       <c r="O272" s="34"/>
       <c r="P272" s="34"/>
-      <c r="Q272" s="72" t="str" cm="1">
+      <c r="Q272" s="71" t="str" cm="1">
         <f t="array" ref="Q272">IF(SUMPRODUCT(--(B272:E272&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -21092,7 +21089,7 @@
       </c>
       <c r="O273" s="34"/>
       <c r="P273" s="34"/>
-      <c r="Q273" s="72" t="str" cm="1">
+      <c r="Q273" s="71" t="str" cm="1">
         <f t="array" ref="Q273">IF(SUMPRODUCT(--(B273:E273&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -21156,7 +21153,7 @@
       </c>
       <c r="O274" s="34"/>
       <c r="P274" s="34"/>
-      <c r="Q274" s="72" t="str" cm="1">
+      <c r="Q274" s="71" t="str" cm="1">
         <f t="array" ref="Q274">IF(SUMPRODUCT(--(B274:E274&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -21220,7 +21217,7 @@
       </c>
       <c r="O275" s="34"/>
       <c r="P275" s="34"/>
-      <c r="Q275" s="72" t="str" cm="1">
+      <c r="Q275" s="71" t="str" cm="1">
         <f t="array" ref="Q275">IF(SUMPRODUCT(--(B275:E275&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -21284,7 +21281,7 @@
       </c>
       <c r="O276" s="34"/>
       <c r="P276" s="34"/>
-      <c r="Q276" s="72" t="str" cm="1">
+      <c r="Q276" s="71" t="str" cm="1">
         <f t="array" ref="Q276">IF(SUMPRODUCT(--(B276:E276&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -21348,7 +21345,7 @@
       </c>
       <c r="O277" s="34"/>
       <c r="P277" s="34"/>
-      <c r="Q277" s="72" t="str" cm="1">
+      <c r="Q277" s="71" t="str" cm="1">
         <f t="array" ref="Q277">IF(SUMPRODUCT(--(B277:E277&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -21412,7 +21409,7 @@
       </c>
       <c r="O278" s="34"/>
       <c r="P278" s="34"/>
-      <c r="Q278" s="72" t="str" cm="1">
+      <c r="Q278" s="71" t="str" cm="1">
         <f t="array" ref="Q278">IF(SUMPRODUCT(--(B278:E278&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -21476,7 +21473,7 @@
       </c>
       <c r="O279" s="34"/>
       <c r="P279" s="34"/>
-      <c r="Q279" s="72" t="str" cm="1">
+      <c r="Q279" s="71" t="str" cm="1">
         <f t="array" ref="Q279">IF(SUMPRODUCT(--(B279:E279&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -21540,7 +21537,7 @@
       </c>
       <c r="O280" s="34"/>
       <c r="P280" s="34"/>
-      <c r="Q280" s="72" t="str" cm="1">
+      <c r="Q280" s="71" t="str" cm="1">
         <f t="array" ref="Q280">IF(SUMPRODUCT(--(B280:E280&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -21604,7 +21601,7 @@
       </c>
       <c r="O281" s="34"/>
       <c r="P281" s="34"/>
-      <c r="Q281" s="72" t="str" cm="1">
+      <c r="Q281" s="71" t="str" cm="1">
         <f t="array" ref="Q281">IF(SUMPRODUCT(--(B281:E281&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -21668,7 +21665,7 @@
       </c>
       <c r="O282" s="34"/>
       <c r="P282" s="34"/>
-      <c r="Q282" s="72" t="str" cm="1">
+      <c r="Q282" s="71" t="str" cm="1">
         <f t="array" ref="Q282">IF(SUMPRODUCT(--(B282:E282&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -21732,7 +21729,7 @@
       </c>
       <c r="O283" s="34"/>
       <c r="P283" s="34"/>
-      <c r="Q283" s="72" t="str" cm="1">
+      <c r="Q283" s="71" t="str" cm="1">
         <f t="array" ref="Q283">IF(SUMPRODUCT(--(B283:E283&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -21796,7 +21793,7 @@
       </c>
       <c r="O284" s="34"/>
       <c r="P284" s="34"/>
-      <c r="Q284" s="72" t="str" cm="1">
+      <c r="Q284" s="71" t="str" cm="1">
         <f t="array" ref="Q284">IF(SUMPRODUCT(--(B284:E284&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -21860,7 +21857,7 @@
       </c>
       <c r="O285" s="34"/>
       <c r="P285" s="34"/>
-      <c r="Q285" s="72" t="str" cm="1">
+      <c r="Q285" s="71" t="str" cm="1">
         <f t="array" ref="Q285">IF(SUMPRODUCT(--(B285:E285&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -21924,7 +21921,7 @@
       </c>
       <c r="O286" s="34"/>
       <c r="P286" s="34"/>
-      <c r="Q286" s="72" t="str" cm="1">
+      <c r="Q286" s="71" t="str" cm="1">
         <f t="array" ref="Q286">IF(SUMPRODUCT(--(B286:E286&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -21988,7 +21985,7 @@
       </c>
       <c r="O287" s="34"/>
       <c r="P287" s="34"/>
-      <c r="Q287" s="72" t="str" cm="1">
+      <c r="Q287" s="71" t="str" cm="1">
         <f t="array" ref="Q287">IF(SUMPRODUCT(--(B287:E287&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -22052,7 +22049,7 @@
       </c>
       <c r="O288" s="34"/>
       <c r="P288" s="34"/>
-      <c r="Q288" s="72" t="str" cm="1">
+      <c r="Q288" s="71" t="str" cm="1">
         <f t="array" ref="Q288">IF(SUMPRODUCT(--(B288:E288&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -22116,7 +22113,7 @@
       </c>
       <c r="O289" s="34"/>
       <c r="P289" s="34"/>
-      <c r="Q289" s="72" t="str" cm="1">
+      <c r="Q289" s="71" t="str" cm="1">
         <f t="array" ref="Q289">IF(SUMPRODUCT(--(B289:E289&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -22180,7 +22177,7 @@
       </c>
       <c r="O290" s="34"/>
       <c r="P290" s="34"/>
-      <c r="Q290" s="72" t="str" cm="1">
+      <c r="Q290" s="71" t="str" cm="1">
         <f t="array" ref="Q290">IF(SUMPRODUCT(--(B290:E290&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -22244,7 +22241,7 @@
       </c>
       <c r="O291" s="34"/>
       <c r="P291" s="34"/>
-      <c r="Q291" s="72" t="str" cm="1">
+      <c r="Q291" s="71" t="str" cm="1">
         <f t="array" ref="Q291">IF(SUMPRODUCT(--(B291:E291&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -22308,7 +22305,7 @@
       </c>
       <c r="O292" s="34"/>
       <c r="P292" s="34"/>
-      <c r="Q292" s="72" t="str" cm="1">
+      <c r="Q292" s="71" t="str" cm="1">
         <f t="array" ref="Q292">IF(SUMPRODUCT(--(B292:E292&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -22372,7 +22369,7 @@
       </c>
       <c r="O293" s="34"/>
       <c r="P293" s="34"/>
-      <c r="Q293" s="72" t="str" cm="1">
+      <c r="Q293" s="71" t="str" cm="1">
         <f t="array" ref="Q293">IF(SUMPRODUCT(--(B293:E293&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -22436,7 +22433,7 @@
       </c>
       <c r="O294" s="34"/>
       <c r="P294" s="34"/>
-      <c r="Q294" s="72" t="str" cm="1">
+      <c r="Q294" s="71" t="str" cm="1">
         <f t="array" ref="Q294">IF(SUMPRODUCT(--(B294:E294&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -22500,7 +22497,7 @@
       </c>
       <c r="O295" s="34"/>
       <c r="P295" s="34"/>
-      <c r="Q295" s="72" t="str" cm="1">
+      <c r="Q295" s="71" t="str" cm="1">
         <f t="array" ref="Q295">IF(SUMPRODUCT(--(B295:E295&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -22564,7 +22561,7 @@
       </c>
       <c r="O296" s="34"/>
       <c r="P296" s="34"/>
-      <c r="Q296" s="72" t="str" cm="1">
+      <c r="Q296" s="71" t="str" cm="1">
         <f t="array" ref="Q296">IF(SUMPRODUCT(--(B296:E296&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -22628,7 +22625,7 @@
       </c>
       <c r="O297" s="34"/>
       <c r="P297" s="34"/>
-      <c r="Q297" s="72" t="str" cm="1">
+      <c r="Q297" s="71" t="str" cm="1">
         <f t="array" ref="Q297">IF(SUMPRODUCT(--(B297:E297&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -22692,7 +22689,7 @@
       </c>
       <c r="O298" s="34"/>
       <c r="P298" s="34"/>
-      <c r="Q298" s="72" t="str" cm="1">
+      <c r="Q298" s="71" t="str" cm="1">
         <f t="array" ref="Q298">IF(SUMPRODUCT(--(B298:E298&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -22756,7 +22753,7 @@
       </c>
       <c r="O299" s="34"/>
       <c r="P299" s="34"/>
-      <c r="Q299" s="72" t="str" cm="1">
+      <c r="Q299" s="71" t="str" cm="1">
         <f t="array" ref="Q299">IF(SUMPRODUCT(--(B299:E299&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -22820,7 +22817,7 @@
       </c>
       <c r="O300" s="34"/>
       <c r="P300" s="34"/>
-      <c r="Q300" s="72" t="str" cm="1">
+      <c r="Q300" s="71" t="str" cm="1">
         <f t="array" ref="Q300">IF(SUMPRODUCT(--(B300:E300&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -22884,7 +22881,7 @@
       </c>
       <c r="O301" s="34"/>
       <c r="P301" s="34"/>
-      <c r="Q301" s="72" t="str" cm="1">
+      <c r="Q301" s="71" t="str" cm="1">
         <f t="array" ref="Q301">IF(SUMPRODUCT(--(B301:E301&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -22948,7 +22945,7 @@
       </c>
       <c r="O302" s="34"/>
       <c r="P302" s="34"/>
-      <c r="Q302" s="72" t="str" cm="1">
+      <c r="Q302" s="71" t="str" cm="1">
         <f t="array" ref="Q302">IF(SUMPRODUCT(--(B302:E302&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -23012,7 +23009,7 @@
       </c>
       <c r="O303" s="34"/>
       <c r="P303" s="34"/>
-      <c r="Q303" s="72" t="str" cm="1">
+      <c r="Q303" s="71" t="str" cm="1">
         <f t="array" ref="Q303">IF(SUMPRODUCT(--(B303:E303&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -23076,7 +23073,7 @@
       </c>
       <c r="O304" s="34"/>
       <c r="P304" s="34"/>
-      <c r="Q304" s="72" t="str" cm="1">
+      <c r="Q304" s="71" t="str" cm="1">
         <f t="array" ref="Q304">IF(SUMPRODUCT(--(B304:E304&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -23140,7 +23137,7 @@
       </c>
       <c r="O305" s="34"/>
       <c r="P305" s="34"/>
-      <c r="Q305" s="72" t="str" cm="1">
+      <c r="Q305" s="71" t="str" cm="1">
         <f t="array" ref="Q305">IF(SUMPRODUCT(--(B305:E305&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -23204,7 +23201,7 @@
       </c>
       <c r="O306" s="34"/>
       <c r="P306" s="34"/>
-      <c r="Q306" s="72" t="str" cm="1">
+      <c r="Q306" s="71" t="str" cm="1">
         <f t="array" ref="Q306">IF(SUMPRODUCT(--(B306:E306&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -23268,7 +23265,7 @@
       </c>
       <c r="O307" s="34"/>
       <c r="P307" s="34"/>
-      <c r="Q307" s="72" t="str" cm="1">
+      <c r="Q307" s="71" t="str" cm="1">
         <f t="array" ref="Q307">IF(SUMPRODUCT(--(B307:E307&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -23332,7 +23329,7 @@
       </c>
       <c r="O308" s="34"/>
       <c r="P308" s="34"/>
-      <c r="Q308" s="72" t="str" cm="1">
+      <c r="Q308" s="71" t="str" cm="1">
         <f t="array" ref="Q308">IF(SUMPRODUCT(--(B308:E308&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -23396,7 +23393,7 @@
       </c>
       <c r="O309" s="34"/>
       <c r="P309" s="34"/>
-      <c r="Q309" s="72" t="str" cm="1">
+      <c r="Q309" s="71" t="str" cm="1">
         <f t="array" ref="Q309">IF(SUMPRODUCT(--(B309:E309&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -23460,7 +23457,7 @@
       </c>
       <c r="O310" s="34"/>
       <c r="P310" s="34"/>
-      <c r="Q310" s="72" t="str" cm="1">
+      <c r="Q310" s="71" t="str" cm="1">
         <f t="array" ref="Q310">IF(SUMPRODUCT(--(B310:E310&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -23524,7 +23521,7 @@
       </c>
       <c r="O311" s="34"/>
       <c r="P311" s="34"/>
-      <c r="Q311" s="72" t="str" cm="1">
+      <c r="Q311" s="71" t="str" cm="1">
         <f t="array" ref="Q311">IF(SUMPRODUCT(--(B311:E311&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -23588,7 +23585,7 @@
       </c>
       <c r="O312" s="34"/>
       <c r="P312" s="34"/>
-      <c r="Q312" s="72" t="str" cm="1">
+      <c r="Q312" s="71" t="str" cm="1">
         <f t="array" ref="Q312">IF(SUMPRODUCT(--(B312:E312&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -23652,7 +23649,7 @@
       </c>
       <c r="O313" s="34"/>
       <c r="P313" s="34"/>
-      <c r="Q313" s="72" t="str" cm="1">
+      <c r="Q313" s="71" t="str" cm="1">
         <f t="array" ref="Q313">IF(SUMPRODUCT(--(B313:E313&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -23716,7 +23713,7 @@
       </c>
       <c r="O314" s="34"/>
       <c r="P314" s="34"/>
-      <c r="Q314" s="72" t="str" cm="1">
+      <c r="Q314" s="71" t="str" cm="1">
         <f t="array" ref="Q314">IF(SUMPRODUCT(--(B314:E314&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -23780,7 +23777,7 @@
       </c>
       <c r="O315" s="34"/>
       <c r="P315" s="34"/>
-      <c r="Q315" s="72" t="str" cm="1">
+      <c r="Q315" s="71" t="str" cm="1">
         <f t="array" ref="Q315">IF(SUMPRODUCT(--(B315:E315&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -23844,7 +23841,7 @@
       </c>
       <c r="O316" s="34"/>
       <c r="P316" s="34"/>
-      <c r="Q316" s="72" t="str" cm="1">
+      <c r="Q316" s="71" t="str" cm="1">
         <f t="array" ref="Q316">IF(SUMPRODUCT(--(B316:E316&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -23908,7 +23905,7 @@
       </c>
       <c r="O317" s="34"/>
       <c r="P317" s="34"/>
-      <c r="Q317" s="72" t="str" cm="1">
+      <c r="Q317" s="71" t="str" cm="1">
         <f t="array" ref="Q317">IF(SUMPRODUCT(--(B317:E317&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -23972,7 +23969,7 @@
       </c>
       <c r="O318" s="34"/>
       <c r="P318" s="34"/>
-      <c r="Q318" s="72" t="str" cm="1">
+      <c r="Q318" s="71" t="str" cm="1">
         <f t="array" ref="Q318">IF(SUMPRODUCT(--(B318:E318&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -24036,7 +24033,7 @@
       </c>
       <c r="O319" s="34"/>
       <c r="P319" s="34"/>
-      <c r="Q319" s="72" t="str" cm="1">
+      <c r="Q319" s="71" t="str" cm="1">
         <f t="array" ref="Q319">IF(SUMPRODUCT(--(B319:E319&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -24100,7 +24097,7 @@
       </c>
       <c r="O320" s="34"/>
       <c r="P320" s="34"/>
-      <c r="Q320" s="72" t="str" cm="1">
+      <c r="Q320" s="71" t="str" cm="1">
         <f t="array" ref="Q320">IF(SUMPRODUCT(--(B320:E320&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -24164,7 +24161,7 @@
       </c>
       <c r="O321" s="34"/>
       <c r="P321" s="34"/>
-      <c r="Q321" s="72" t="str" cm="1">
+      <c r="Q321" s="71" t="str" cm="1">
         <f t="array" ref="Q321">IF(SUMPRODUCT(--(B321:E321&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -24228,7 +24225,7 @@
       </c>
       <c r="O322" s="34"/>
       <c r="P322" s="34"/>
-      <c r="Q322" s="72" t="str" cm="1">
+      <c r="Q322" s="71" t="str" cm="1">
         <f t="array" ref="Q322">IF(SUMPRODUCT(--(B322:E322&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -24292,7 +24289,7 @@
       </c>
       <c r="O323" s="34"/>
       <c r="P323" s="34"/>
-      <c r="Q323" s="72" t="str" cm="1">
+      <c r="Q323" s="71" t="str" cm="1">
         <f t="array" ref="Q323">IF(SUMPRODUCT(--(B323:E323&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -24356,7 +24353,7 @@
       </c>
       <c r="O324" s="34"/>
       <c r="P324" s="34"/>
-      <c r="Q324" s="72" t="str" cm="1">
+      <c r="Q324" s="71" t="str" cm="1">
         <f t="array" ref="Q324">IF(SUMPRODUCT(--(B324:E324&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -24420,7 +24417,7 @@
       </c>
       <c r="O325" s="34"/>
       <c r="P325" s="34"/>
-      <c r="Q325" s="72" t="str" cm="1">
+      <c r="Q325" s="71" t="str" cm="1">
         <f t="array" ref="Q325">IF(SUMPRODUCT(--(B325:E325&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -24484,7 +24481,7 @@
       </c>
       <c r="O326" s="34"/>
       <c r="P326" s="34"/>
-      <c r="Q326" s="72" t="str" cm="1">
+      <c r="Q326" s="71" t="str" cm="1">
         <f t="array" ref="Q326">IF(SUMPRODUCT(--(B326:E326&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -24548,7 +24545,7 @@
       </c>
       <c r="O327" s="34"/>
       <c r="P327" s="34"/>
-      <c r="Q327" s="72" t="str" cm="1">
+      <c r="Q327" s="71" t="str" cm="1">
         <f t="array" ref="Q327">IF(SUMPRODUCT(--(B327:E327&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -24612,7 +24609,7 @@
       </c>
       <c r="O328" s="34"/>
       <c r="P328" s="34"/>
-      <c r="Q328" s="72" t="str" cm="1">
+      <c r="Q328" s="71" t="str" cm="1">
         <f t="array" ref="Q328">IF(SUMPRODUCT(--(B328:E328&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -24676,7 +24673,7 @@
       </c>
       <c r="O329" s="34"/>
       <c r="P329" s="34"/>
-      <c r="Q329" s="72" t="str" cm="1">
+      <c r="Q329" s="71" t="str" cm="1">
         <f t="array" ref="Q329">IF(SUMPRODUCT(--(B329:E329&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -24740,7 +24737,7 @@
       </c>
       <c r="O330" s="34"/>
       <c r="P330" s="34"/>
-      <c r="Q330" s="72" t="str" cm="1">
+      <c r="Q330" s="71" t="str" cm="1">
         <f t="array" ref="Q330">IF(SUMPRODUCT(--(B330:E330&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -24804,7 +24801,7 @@
       </c>
       <c r="O331" s="34"/>
       <c r="P331" s="34"/>
-      <c r="Q331" s="72" t="str" cm="1">
+      <c r="Q331" s="71" t="str" cm="1">
         <f t="array" ref="Q331">IF(SUMPRODUCT(--(B331:E331&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -24868,7 +24865,7 @@
       </c>
       <c r="O332" s="34"/>
       <c r="P332" s="34"/>
-      <c r="Q332" s="72" t="str" cm="1">
+      <c r="Q332" s="71" t="str" cm="1">
         <f t="array" ref="Q332">IF(SUMPRODUCT(--(B332:E332&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -24932,7 +24929,7 @@
       </c>
       <c r="O333" s="34"/>
       <c r="P333" s="34"/>
-      <c r="Q333" s="72" t="str" cm="1">
+      <c r="Q333" s="71" t="str" cm="1">
         <f t="array" ref="Q333">IF(SUMPRODUCT(--(B333:E333&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -24996,7 +24993,7 @@
       </c>
       <c r="O334" s="34"/>
       <c r="P334" s="34"/>
-      <c r="Q334" s="72" t="str" cm="1">
+      <c r="Q334" s="71" t="str" cm="1">
         <f t="array" ref="Q334">IF(SUMPRODUCT(--(B334:E334&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -25060,7 +25057,7 @@
       </c>
       <c r="O335" s="34"/>
       <c r="P335" s="34"/>
-      <c r="Q335" s="72" t="str" cm="1">
+      <c r="Q335" s="71" t="str" cm="1">
         <f t="array" ref="Q335">IF(SUMPRODUCT(--(B335:E335&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -25124,7 +25121,7 @@
       </c>
       <c r="O336" s="34"/>
       <c r="P336" s="34"/>
-      <c r="Q336" s="72" t="str" cm="1">
+      <c r="Q336" s="71" t="str" cm="1">
         <f t="array" ref="Q336">IF(SUMPRODUCT(--(B336:E336&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -25188,7 +25185,7 @@
       </c>
       <c r="O337" s="34"/>
       <c r="P337" s="34"/>
-      <c r="Q337" s="72" t="str" cm="1">
+      <c r="Q337" s="71" t="str" cm="1">
         <f t="array" ref="Q337">IF(SUMPRODUCT(--(B337:E337&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -25252,7 +25249,7 @@
       </c>
       <c r="O338" s="34"/>
       <c r="P338" s="34"/>
-      <c r="Q338" s="72" t="str" cm="1">
+      <c r="Q338" s="71" t="str" cm="1">
         <f t="array" ref="Q338">IF(SUMPRODUCT(--(B338:E338&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -25316,7 +25313,7 @@
       </c>
       <c r="O339" s="34"/>
       <c r="P339" s="34"/>
-      <c r="Q339" s="72" t="str" cm="1">
+      <c r="Q339" s="71" t="str" cm="1">
         <f t="array" ref="Q339">IF(SUMPRODUCT(--(B339:E339&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -25380,7 +25377,7 @@
       </c>
       <c r="O340" s="34"/>
       <c r="P340" s="34"/>
-      <c r="Q340" s="72" t="str" cm="1">
+      <c r="Q340" s="71" t="str" cm="1">
         <f t="array" ref="Q340">IF(SUMPRODUCT(--(B340:E340&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -25444,7 +25441,7 @@
       </c>
       <c r="O341" s="34"/>
       <c r="P341" s="34"/>
-      <c r="Q341" s="72" t="str" cm="1">
+      <c r="Q341" s="71" t="str" cm="1">
         <f t="array" ref="Q341">IF(SUMPRODUCT(--(B341:E341&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -25508,7 +25505,7 @@
       </c>
       <c r="O342" s="34"/>
       <c r="P342" s="34"/>
-      <c r="Q342" s="72" t="str" cm="1">
+      <c r="Q342" s="71" t="str" cm="1">
         <f t="array" ref="Q342">IF(SUMPRODUCT(--(B342:E342&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -25572,7 +25569,7 @@
       </c>
       <c r="O343" s="34"/>
       <c r="P343" s="34"/>
-      <c r="Q343" s="72" t="str" cm="1">
+      <c r="Q343" s="71" t="str" cm="1">
         <f t="array" ref="Q343">IF(SUMPRODUCT(--(B343:E343&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -25636,7 +25633,7 @@
       </c>
       <c r="O344" s="34"/>
       <c r="P344" s="34"/>
-      <c r="Q344" s="72" t="str" cm="1">
+      <c r="Q344" s="71" t="str" cm="1">
         <f t="array" ref="Q344">IF(SUMPRODUCT(--(B344:E344&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -25700,7 +25697,7 @@
       </c>
       <c r="O345" s="34"/>
       <c r="P345" s="34"/>
-      <c r="Q345" s="72" t="str" cm="1">
+      <c r="Q345" s="71" t="str" cm="1">
         <f t="array" ref="Q345">IF(SUMPRODUCT(--(B345:E345&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -25764,7 +25761,7 @@
       </c>
       <c r="O346" s="34"/>
       <c r="P346" s="34"/>
-      <c r="Q346" s="72" t="str" cm="1">
+      <c r="Q346" s="71" t="str" cm="1">
         <f t="array" ref="Q346">IF(SUMPRODUCT(--(B346:E346&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -25828,7 +25825,7 @@
       </c>
       <c r="O347" s="34"/>
       <c r="P347" s="34"/>
-      <c r="Q347" s="72" t="str" cm="1">
+      <c r="Q347" s="71" t="str" cm="1">
         <f t="array" ref="Q347">IF(SUMPRODUCT(--(B347:E347&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -25892,7 +25889,7 @@
       </c>
       <c r="O348" s="34"/>
       <c r="P348" s="34"/>
-      <c r="Q348" s="72" t="str" cm="1">
+      <c r="Q348" s="71" t="str" cm="1">
         <f t="array" ref="Q348">IF(SUMPRODUCT(--(B348:E348&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -25956,7 +25953,7 @@
       </c>
       <c r="O349" s="34"/>
       <c r="P349" s="34"/>
-      <c r="Q349" s="72" t="str" cm="1">
+      <c r="Q349" s="71" t="str" cm="1">
         <f t="array" ref="Q349">IF(SUMPRODUCT(--(B349:E349&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -26020,7 +26017,7 @@
       </c>
       <c r="O350" s="34"/>
       <c r="P350" s="34"/>
-      <c r="Q350" s="72" t="str" cm="1">
+      <c r="Q350" s="71" t="str" cm="1">
         <f t="array" ref="Q350">IF(SUMPRODUCT(--(B350:E350&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -26084,7 +26081,7 @@
       </c>
       <c r="O351" s="34"/>
       <c r="P351" s="34"/>
-      <c r="Q351" s="72" t="str" cm="1">
+      <c r="Q351" s="71" t="str" cm="1">
         <f t="array" ref="Q351">IF(SUMPRODUCT(--(B351:E351&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -26148,7 +26145,7 @@
       </c>
       <c r="O352" s="34"/>
       <c r="P352" s="34"/>
-      <c r="Q352" s="72" t="str" cm="1">
+      <c r="Q352" s="71" t="str" cm="1">
         <f t="array" ref="Q352">IF(SUMPRODUCT(--(B352:E352&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -26212,7 +26209,7 @@
       </c>
       <c r="O353" s="34"/>
       <c r="P353" s="34"/>
-      <c r="Q353" s="72" t="str" cm="1">
+      <c r="Q353" s="71" t="str" cm="1">
         <f t="array" ref="Q353">IF(SUMPRODUCT(--(B353:E353&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -26276,7 +26273,7 @@
       </c>
       <c r="O354" s="34"/>
       <c r="P354" s="34"/>
-      <c r="Q354" s="72" t="str" cm="1">
+      <c r="Q354" s="71" t="str" cm="1">
         <f t="array" ref="Q354">IF(SUMPRODUCT(--(B354:E354&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -26340,7 +26337,7 @@
       </c>
       <c r="O355" s="34"/>
       <c r="P355" s="34"/>
-      <c r="Q355" s="72" t="str" cm="1">
+      <c r="Q355" s="71" t="str" cm="1">
         <f t="array" ref="Q355">IF(SUMPRODUCT(--(B355:E355&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -26404,7 +26401,7 @@
       </c>
       <c r="O356" s="34"/>
       <c r="P356" s="34"/>
-      <c r="Q356" s="72" t="str" cm="1">
+      <c r="Q356" s="71" t="str" cm="1">
         <f t="array" ref="Q356">IF(SUMPRODUCT(--(B356:E356&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -26468,7 +26465,7 @@
       </c>
       <c r="O357" s="34"/>
       <c r="P357" s="34"/>
-      <c r="Q357" s="72" t="str" cm="1">
+      <c r="Q357" s="71" t="str" cm="1">
         <f t="array" ref="Q357">IF(SUMPRODUCT(--(B357:E357&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -26532,7 +26529,7 @@
       </c>
       <c r="O358" s="34"/>
       <c r="P358" s="34"/>
-      <c r="Q358" s="72" t="str" cm="1">
+      <c r="Q358" s="71" t="str" cm="1">
         <f t="array" ref="Q358">IF(SUMPRODUCT(--(B358:E358&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -26596,7 +26593,7 @@
       </c>
       <c r="O359" s="34"/>
       <c r="P359" s="34"/>
-      <c r="Q359" s="72" t="str" cm="1">
+      <c r="Q359" s="71" t="str" cm="1">
         <f t="array" ref="Q359">IF(SUMPRODUCT(--(B359:E359&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -26660,7 +26657,7 @@
       </c>
       <c r="O360" s="34"/>
       <c r="P360" s="34"/>
-      <c r="Q360" s="72" t="str" cm="1">
+      <c r="Q360" s="71" t="str" cm="1">
         <f t="array" ref="Q360">IF(SUMPRODUCT(--(B360:E360&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -26724,7 +26721,7 @@
       </c>
       <c r="O361" s="34"/>
       <c r="P361" s="34"/>
-      <c r="Q361" s="72" t="str" cm="1">
+      <c r="Q361" s="71" t="str" cm="1">
         <f t="array" ref="Q361">IF(SUMPRODUCT(--(B361:E361&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -26788,7 +26785,7 @@
       </c>
       <c r="O362" s="34"/>
       <c r="P362" s="34"/>
-      <c r="Q362" s="72" t="str" cm="1">
+      <c r="Q362" s="71" t="str" cm="1">
         <f t="array" ref="Q362">IF(SUMPRODUCT(--(B362:E362&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -26852,7 +26849,7 @@
       </c>
       <c r="O363" s="34"/>
       <c r="P363" s="34"/>
-      <c r="Q363" s="72" t="str" cm="1">
+      <c r="Q363" s="71" t="str" cm="1">
         <f t="array" ref="Q363">IF(SUMPRODUCT(--(B363:E363&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -26916,7 +26913,7 @@
       </c>
       <c r="O364" s="34"/>
       <c r="P364" s="34"/>
-      <c r="Q364" s="72" t="str" cm="1">
+      <c r="Q364" s="71" t="str" cm="1">
         <f t="array" ref="Q364">IF(SUMPRODUCT(--(B364:E364&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -26980,7 +26977,7 @@
       </c>
       <c r="O365" s="34"/>
       <c r="P365" s="34"/>
-      <c r="Q365" s="72" t="str" cm="1">
+      <c r="Q365" s="71" t="str" cm="1">
         <f t="array" ref="Q365">IF(SUMPRODUCT(--(B365:E365&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -27044,7 +27041,7 @@
       </c>
       <c r="O366" s="34"/>
       <c r="P366" s="34"/>
-      <c r="Q366" s="72" t="str" cm="1">
+      <c r="Q366" s="71" t="str" cm="1">
         <f t="array" ref="Q366">IF(SUMPRODUCT(--(B366:E366&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -27108,7 +27105,7 @@
       </c>
       <c r="O367" s="34"/>
       <c r="P367" s="34"/>
-      <c r="Q367" s="72" t="str" cm="1">
+      <c r="Q367" s="71" t="str" cm="1">
         <f t="array" ref="Q367">IF(SUMPRODUCT(--(B367:E367&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -27172,7 +27169,7 @@
       </c>
       <c r="O368" s="34"/>
       <c r="P368" s="34"/>
-      <c r="Q368" s="72" t="str" cm="1">
+      <c r="Q368" s="71" t="str" cm="1">
         <f t="array" ref="Q368">IF(SUMPRODUCT(--(B368:E368&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -27236,7 +27233,7 @@
       </c>
       <c r="O369" s="34"/>
       <c r="P369" s="34"/>
-      <c r="Q369" s="72" t="str" cm="1">
+      <c r="Q369" s="71" t="str" cm="1">
         <f t="array" ref="Q369">IF(SUMPRODUCT(--(B369:E369&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -27300,7 +27297,7 @@
       </c>
       <c r="O370" s="34"/>
       <c r="P370" s="34"/>
-      <c r="Q370" s="72" t="str" cm="1">
+      <c r="Q370" s="71" t="str" cm="1">
         <f t="array" ref="Q370">IF(SUMPRODUCT(--(B370:E370&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -27364,7 +27361,7 @@
       </c>
       <c r="O371" s="34"/>
       <c r="P371" s="34"/>
-      <c r="Q371" s="72" t="str" cm="1">
+      <c r="Q371" s="71" t="str" cm="1">
         <f t="array" ref="Q371">IF(SUMPRODUCT(--(B371:E371&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -27428,7 +27425,7 @@
       </c>
       <c r="O372" s="34"/>
       <c r="P372" s="34"/>
-      <c r="Q372" s="72" t="str" cm="1">
+      <c r="Q372" s="71" t="str" cm="1">
         <f t="array" ref="Q372">IF(SUMPRODUCT(--(B372:E372&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -27492,7 +27489,7 @@
       </c>
       <c r="O373" s="34"/>
       <c r="P373" s="34"/>
-      <c r="Q373" s="72" t="str" cm="1">
+      <c r="Q373" s="71" t="str" cm="1">
         <f t="array" ref="Q373">IF(SUMPRODUCT(--(B373:E373&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -27556,7 +27553,7 @@
       </c>
       <c r="O374" s="34"/>
       <c r="P374" s="34"/>
-      <c r="Q374" s="72" t="str" cm="1">
+      <c r="Q374" s="71" t="str" cm="1">
         <f t="array" ref="Q374">IF(SUMPRODUCT(--(B374:E374&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -27620,7 +27617,7 @@
       </c>
       <c r="O375" s="34"/>
       <c r="P375" s="34"/>
-      <c r="Q375" s="72" t="str" cm="1">
+      <c r="Q375" s="71" t="str" cm="1">
         <f t="array" ref="Q375">IF(SUMPRODUCT(--(B375:E375&lt;&gt;""))&gt;0,"○","")</f>
         <v/>
       </c>
@@ -27671,7 +27668,7 @@
       <c r="N376" s="41"/>
       <c r="O376" s="40"/>
       <c r="P376" s="40"/>
-      <c r="Q376" s="73"/>
+      <c r="Q376" s="72"/>
       <c r="R376" s="42"/>
       <c r="S376" s="42"/>
       <c r="T376" s="42"/>
@@ -27686,7 +27683,7 @@
     <row r="378" spans="1:268" x14ac:dyDescent="0.4">
       <c r="O378" s="47"/>
       <c r="P378" s="47"/>
-      <c r="Q378" s="74"/>
+      <c r="Q378" s="73"/>
       <c r="R378" s="48"/>
       <c r="S378" s="48"/>
       <c r="T378" s="48"/>
@@ -27694,7 +27691,7 @@
     <row r="379" spans="1:268" x14ac:dyDescent="0.4">
       <c r="O379" s="49"/>
       <c r="P379" s="49"/>
-      <c r="Q379" s="75"/>
+      <c r="Q379" s="74"/>
       <c r="R379" s="50"/>
       <c r="S379" s="50"/>
       <c r="T379" s="50"/>

</xml_diff>